<commit_message>
May 11 Figure Update
</commit_message>
<xml_diff>
--- a/PXD020586/sdrf.xlsx
+++ b/PXD020586/sdrf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Payne Lab\TMT\TMT_QC\PXD020586\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7531B-DD3C-400F-BE58-3D57F692336B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD88E175-63DA-4741-BD64-97959C3A8B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B0FF2B6B-E326-450E-82DA-7E4299F0AAC8}"/>
   </bookViews>
@@ -414,7 +414,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,12 +427,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,12 +449,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0AE791-64B6-4DAB-A49D-D63DB87399C3}">
   <dimension ref="A1:J1428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1340" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1354" sqref="D1354"/>
     </sheetView>
   </sheetViews>
@@ -15688,7 +15681,7 @@
       </c>
     </row>
     <row r="495" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A495" s="2" t="s">
+      <c r="A495" t="s">
         <v>61</v>
       </c>
       <c r="B495" t="s">
@@ -15720,7 +15713,7 @@
       </c>
     </row>
     <row r="496" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A496" s="2" t="s">
+      <c r="A496" t="s">
         <v>61</v>
       </c>
       <c r="B496" t="s">
@@ -15752,7 +15745,7 @@
       </c>
     </row>
     <row r="497" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A497" s="2" t="s">
+      <c r="A497" t="s">
         <v>61</v>
       </c>
       <c r="B497" t="s">
@@ -15784,7 +15777,7 @@
       </c>
     </row>
     <row r="498" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A498" s="2" t="s">
+      <c r="A498" t="s">
         <v>61</v>
       </c>
       <c r="B498" t="s">
@@ -15816,7 +15809,7 @@
       </c>
     </row>
     <row r="499" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A499" s="2" t="s">
+      <c r="A499" t="s">
         <v>61</v>
       </c>
       <c r="B499" t="s">
@@ -15848,7 +15841,7 @@
       </c>
     </row>
     <row r="500" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A500" s="2" t="s">
+      <c r="A500" t="s">
         <v>61</v>
       </c>
       <c r="B500" t="s">
@@ -15880,7 +15873,7 @@
       </c>
     </row>
     <row r="501" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A501" s="2" t="s">
+      <c r="A501" t="s">
         <v>61</v>
       </c>
       <c r="B501" t="s">
@@ -15912,7 +15905,7 @@
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A502" s="2" t="s">
+      <c r="A502" t="s">
         <v>61</v>
       </c>
       <c r="B502" t="s">
@@ -15944,7 +15937,7 @@
       </c>
     </row>
     <row r="503" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A503" s="2" t="s">
+      <c r="A503" t="s">
         <v>61</v>
       </c>
       <c r="B503" t="s">
@@ -15976,7 +15969,7 @@
       </c>
     </row>
     <row r="504" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A504" s="2" t="s">
+      <c r="A504" t="s">
         <v>61</v>
       </c>
       <c r="B504" t="s">
@@ -16008,7 +16001,7 @@
       </c>
     </row>
     <row r="505" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A505" s="2" t="s">
+      <c r="A505" t="s">
         <v>61</v>
       </c>
       <c r="B505" t="s">
@@ -16040,7 +16033,7 @@
       </c>
     </row>
     <row r="506" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A506" s="2" t="s">
+      <c r="A506" t="s">
         <v>61</v>
       </c>
       <c r="B506" t="s">
@@ -16072,7 +16065,7 @@
       </c>
     </row>
     <row r="507" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A507" s="2" t="s">
+      <c r="A507" t="s">
         <v>61</v>
       </c>
       <c r="B507" t="s">
@@ -16104,7 +16097,7 @@
       </c>
     </row>
     <row r="508" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A508" s="2" t="s">
+      <c r="A508" t="s">
         <v>61</v>
       </c>
       <c r="B508" t="s">
@@ -16136,7 +16129,7 @@
       </c>
     </row>
     <row r="509" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A509" s="2" t="s">
+      <c r="A509" t="s">
         <v>61</v>
       </c>
       <c r="B509" t="s">
@@ -16168,7 +16161,7 @@
       </c>
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A510" s="2" t="s">
+      <c r="A510" t="s">
         <v>61</v>
       </c>
       <c r="B510" t="s">
@@ -16200,7 +16193,7 @@
       </c>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A512" s="2" t="s">
+      <c r="A512" t="s">
         <v>62</v>
       </c>
       <c r="B512" t="s">
@@ -16232,7 +16225,7 @@
       </c>
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A513" s="2" t="s">
+      <c r="A513" t="s">
         <v>62</v>
       </c>
       <c r="B513" t="s">
@@ -16264,7 +16257,7 @@
       </c>
     </row>
     <row r="514" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A514" s="2" t="s">
+      <c r="A514" t="s">
         <v>62</v>
       </c>
       <c r="B514" t="s">
@@ -16296,7 +16289,7 @@
       </c>
     </row>
     <row r="515" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A515" s="2" t="s">
+      <c r="A515" t="s">
         <v>62</v>
       </c>
       <c r="B515" t="s">
@@ -16328,7 +16321,7 @@
       </c>
     </row>
     <row r="516" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A516" s="2" t="s">
+      <c r="A516" t="s">
         <v>62</v>
       </c>
       <c r="B516" t="s">
@@ -16360,7 +16353,7 @@
       </c>
     </row>
     <row r="517" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A517" s="2" t="s">
+      <c r="A517" t="s">
         <v>62</v>
       </c>
       <c r="B517" t="s">
@@ -16392,7 +16385,7 @@
       </c>
     </row>
     <row r="518" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A518" s="2" t="s">
+      <c r="A518" t="s">
         <v>62</v>
       </c>
       <c r="B518" t="s">
@@ -16424,7 +16417,7 @@
       </c>
     </row>
     <row r="519" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A519" s="2" t="s">
+      <c r="A519" t="s">
         <v>62</v>
       </c>
       <c r="B519" t="s">
@@ -16456,7 +16449,7 @@
       </c>
     </row>
     <row r="520" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A520" s="2" t="s">
+      <c r="A520" t="s">
         <v>62</v>
       </c>
       <c r="B520" t="s">
@@ -16488,7 +16481,7 @@
       </c>
     </row>
     <row r="521" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A521" s="2" t="s">
+      <c r="A521" t="s">
         <v>62</v>
       </c>
       <c r="B521" t="s">
@@ -16520,7 +16513,7 @@
       </c>
     </row>
     <row r="522" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A522" s="2" t="s">
+      <c r="A522" t="s">
         <v>62</v>
       </c>
       <c r="B522" t="s">
@@ -16552,7 +16545,7 @@
       </c>
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A523" s="2" t="s">
+      <c r="A523" t="s">
         <v>62</v>
       </c>
       <c r="B523" t="s">
@@ -16584,7 +16577,7 @@
       </c>
     </row>
     <row r="524" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A524" s="2" t="s">
+      <c r="A524" t="s">
         <v>62</v>
       </c>
       <c r="B524" t="s">
@@ -16616,7 +16609,7 @@
       </c>
     </row>
     <row r="525" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A525" s="2" t="s">
+      <c r="A525" t="s">
         <v>62</v>
       </c>
       <c r="B525" t="s">
@@ -16648,7 +16641,7 @@
       </c>
     </row>
     <row r="526" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A526" s="2" t="s">
+      <c r="A526" t="s">
         <v>62</v>
       </c>
       <c r="B526" t="s">
@@ -16680,7 +16673,7 @@
       </c>
     </row>
     <row r="527" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A527" s="2" t="s">
+      <c r="A527" t="s">
         <v>62</v>
       </c>
       <c r="B527" t="s">
@@ -16712,7 +16705,7 @@
       </c>
     </row>
     <row r="529" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A529" s="2" t="s">
+      <c r="A529" t="s">
         <v>63</v>
       </c>
       <c r="B529" t="s">
@@ -16744,7 +16737,7 @@
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A530" s="2" t="s">
+      <c r="A530" t="s">
         <v>63</v>
       </c>
       <c r="B530" t="s">
@@ -16776,7 +16769,7 @@
       </c>
     </row>
     <row r="531" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A531" s="2" t="s">
+      <c r="A531" t="s">
         <v>63</v>
       </c>
       <c r="B531" t="s">
@@ -16808,7 +16801,7 @@
       </c>
     </row>
     <row r="532" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A532" s="2" t="s">
+      <c r="A532" t="s">
         <v>63</v>
       </c>
       <c r="B532" t="s">
@@ -16840,7 +16833,7 @@
       </c>
     </row>
     <row r="533" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A533" s="2" t="s">
+      <c r="A533" t="s">
         <v>63</v>
       </c>
       <c r="B533" t="s">
@@ -16872,7 +16865,7 @@
       </c>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A534" s="2" t="s">
+      <c r="A534" t="s">
         <v>63</v>
       </c>
       <c r="B534" t="s">
@@ -16904,7 +16897,7 @@
       </c>
     </row>
     <row r="535" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A535" s="2" t="s">
+      <c r="A535" t="s">
         <v>63</v>
       </c>
       <c r="B535" t="s">
@@ -16936,7 +16929,7 @@
       </c>
     </row>
     <row r="536" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A536" s="2" t="s">
+      <c r="A536" t="s">
         <v>63</v>
       </c>
       <c r="B536" t="s">
@@ -16968,7 +16961,7 @@
       </c>
     </row>
     <row r="537" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A537" s="2" t="s">
+      <c r="A537" t="s">
         <v>63</v>
       </c>
       <c r="B537" t="s">
@@ -17000,7 +16993,7 @@
       </c>
     </row>
     <row r="538" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A538" s="2" t="s">
+      <c r="A538" t="s">
         <v>63</v>
       </c>
       <c r="B538" t="s">
@@ -17032,7 +17025,7 @@
       </c>
     </row>
     <row r="539" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A539" s="2" t="s">
+      <c r="A539" t="s">
         <v>63</v>
       </c>
       <c r="B539" t="s">
@@ -17064,7 +17057,7 @@
       </c>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A540" s="2" t="s">
+      <c r="A540" t="s">
         <v>63</v>
       </c>
       <c r="B540" t="s">
@@ -17096,7 +17089,7 @@
       </c>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A541" s="2" t="s">
+      <c r="A541" t="s">
         <v>63</v>
       </c>
       <c r="B541" t="s">
@@ -17128,7 +17121,7 @@
       </c>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A542" s="2" t="s">
+      <c r="A542" t="s">
         <v>63</v>
       </c>
       <c r="B542" t="s">
@@ -17160,7 +17153,7 @@
       </c>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A543" s="2" t="s">
+      <c r="A543" t="s">
         <v>63</v>
       </c>
       <c r="B543" t="s">
@@ -17192,7 +17185,7 @@
       </c>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A544" s="2" t="s">
+      <c r="A544" t="s">
         <v>63</v>
       </c>
       <c r="B544" t="s">
@@ -17224,7 +17217,7 @@
       </c>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A546" s="2" t="s">
+      <c r="A546" t="s">
         <v>64</v>
       </c>
       <c r="B546" t="s">
@@ -17256,7 +17249,7 @@
       </c>
     </row>
     <row r="547" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A547" s="2" t="s">
+      <c r="A547" t="s">
         <v>64</v>
       </c>
       <c r="B547" t="s">
@@ -17288,7 +17281,7 @@
       </c>
     </row>
     <row r="548" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A548" s="2" t="s">
+      <c r="A548" t="s">
         <v>64</v>
       </c>
       <c r="B548" t="s">
@@ -17320,7 +17313,7 @@
       </c>
     </row>
     <row r="549" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A549" s="2" t="s">
+      <c r="A549" t="s">
         <v>64</v>
       </c>
       <c r="B549" t="s">
@@ -17352,7 +17345,7 @@
       </c>
     </row>
     <row r="550" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A550" s="2" t="s">
+      <c r="A550" t="s">
         <v>64</v>
       </c>
       <c r="B550" t="s">
@@ -17384,7 +17377,7 @@
       </c>
     </row>
     <row r="551" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A551" s="2" t="s">
+      <c r="A551" t="s">
         <v>64</v>
       </c>
       <c r="B551" t="s">
@@ -17416,7 +17409,7 @@
       </c>
     </row>
     <row r="552" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A552" s="2" t="s">
+      <c r="A552" t="s">
         <v>64</v>
       </c>
       <c r="B552" t="s">
@@ -17448,7 +17441,7 @@
       </c>
     </row>
     <row r="553" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A553" s="2" t="s">
+      <c r="A553" t="s">
         <v>64</v>
       </c>
       <c r="B553" t="s">
@@ -17480,7 +17473,7 @@
       </c>
     </row>
     <row r="554" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A554" s="2" t="s">
+      <c r="A554" t="s">
         <v>64</v>
       </c>
       <c r="B554" t="s">
@@ -17512,7 +17505,7 @@
       </c>
     </row>
     <row r="555" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A555" s="2" t="s">
+      <c r="A555" t="s">
         <v>64</v>
       </c>
       <c r="B555" t="s">
@@ -17544,7 +17537,7 @@
       </c>
     </row>
     <row r="556" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A556" s="2" t="s">
+      <c r="A556" t="s">
         <v>64</v>
       </c>
       <c r="B556" t="s">
@@ -17576,7 +17569,7 @@
       </c>
     </row>
     <row r="557" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A557" s="2" t="s">
+      <c r="A557" t="s">
         <v>64</v>
       </c>
       <c r="B557" t="s">
@@ -17608,7 +17601,7 @@
       </c>
     </row>
     <row r="558" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A558" s="2" t="s">
+      <c r="A558" t="s">
         <v>64</v>
       </c>
       <c r="B558" t="s">
@@ -17640,7 +17633,7 @@
       </c>
     </row>
     <row r="559" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A559" s="2" t="s">
+      <c r="A559" t="s">
         <v>64</v>
       </c>
       <c r="B559" t="s">
@@ -17672,7 +17665,7 @@
       </c>
     </row>
     <row r="560" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A560" s="2" t="s">
+      <c r="A560" t="s">
         <v>64</v>
       </c>
       <c r="B560" t="s">
@@ -17704,7 +17697,7 @@
       </c>
     </row>
     <row r="561" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A561" s="2" t="s">
+      <c r="A561" t="s">
         <v>64</v>
       </c>
       <c r="B561" t="s">
@@ -17736,7 +17729,7 @@
       </c>
     </row>
     <row r="563" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A563" s="2" t="s">
+      <c r="A563" t="s">
         <v>65</v>
       </c>
       <c r="B563" t="s">
@@ -17768,7 +17761,7 @@
       </c>
     </row>
     <row r="564" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A564" s="2" t="s">
+      <c r="A564" t="s">
         <v>65</v>
       </c>
       <c r="B564" t="s">
@@ -17800,7 +17793,7 @@
       </c>
     </row>
     <row r="565" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A565" s="2" t="s">
+      <c r="A565" t="s">
         <v>65</v>
       </c>
       <c r="B565" t="s">
@@ -17832,7 +17825,7 @@
       </c>
     </row>
     <row r="566" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A566" s="2" t="s">
+      <c r="A566" t="s">
         <v>65</v>
       </c>
       <c r="B566" t="s">
@@ -17864,7 +17857,7 @@
       </c>
     </row>
     <row r="567" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A567" s="2" t="s">
+      <c r="A567" t="s">
         <v>65</v>
       </c>
       <c r="B567" t="s">
@@ -17896,7 +17889,7 @@
       </c>
     </row>
     <row r="568" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A568" s="2" t="s">
+      <c r="A568" t="s">
         <v>65</v>
       </c>
       <c r="B568" t="s">
@@ -17928,7 +17921,7 @@
       </c>
     </row>
     <row r="569" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A569" s="2" t="s">
+      <c r="A569" t="s">
         <v>65</v>
       </c>
       <c r="B569" t="s">
@@ -17960,7 +17953,7 @@
       </c>
     </row>
     <row r="570" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A570" s="2" t="s">
+      <c r="A570" t="s">
         <v>65</v>
       </c>
       <c r="B570" t="s">
@@ -17992,7 +17985,7 @@
       </c>
     </row>
     <row r="571" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A571" s="2" t="s">
+      <c r="A571" t="s">
         <v>65</v>
       </c>
       <c r="B571" t="s">
@@ -18024,7 +18017,7 @@
       </c>
     </row>
     <row r="572" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A572" s="2" t="s">
+      <c r="A572" t="s">
         <v>65</v>
       </c>
       <c r="B572" t="s">
@@ -18056,7 +18049,7 @@
       </c>
     </row>
     <row r="573" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A573" s="2" t="s">
+      <c r="A573" t="s">
         <v>65</v>
       </c>
       <c r="B573" t="s">
@@ -18088,7 +18081,7 @@
       </c>
     </row>
     <row r="574" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A574" s="2" t="s">
+      <c r="A574" t="s">
         <v>65</v>
       </c>
       <c r="B574" t="s">
@@ -18120,7 +18113,7 @@
       </c>
     </row>
     <row r="575" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A575" s="2" t="s">
+      <c r="A575" t="s">
         <v>65</v>
       </c>
       <c r="B575" t="s">
@@ -18152,7 +18145,7 @@
       </c>
     </row>
     <row r="576" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A576" s="2" t="s">
+      <c r="A576" t="s">
         <v>65</v>
       </c>
       <c r="B576" t="s">
@@ -18184,7 +18177,7 @@
       </c>
     </row>
     <row r="577" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A577" s="2" t="s">
+      <c r="A577" t="s">
         <v>65</v>
       </c>
       <c r="B577" t="s">
@@ -18216,7 +18209,7 @@
       </c>
     </row>
     <row r="578" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A578" s="2" t="s">
+      <c r="A578" t="s">
         <v>65</v>
       </c>
       <c r="B578" t="s">
@@ -18248,7 +18241,7 @@
       </c>
     </row>
     <row r="580" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A580" s="2" t="s">
+      <c r="A580" t="s">
         <v>66</v>
       </c>
       <c r="B580" t="s">
@@ -18280,7 +18273,7 @@
       </c>
     </row>
     <row r="581" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A581" s="2" t="s">
+      <c r="A581" t="s">
         <v>66</v>
       </c>
       <c r="B581" t="s">
@@ -18312,7 +18305,7 @@
       </c>
     </row>
     <row r="582" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A582" s="2" t="s">
+      <c r="A582" t="s">
         <v>66</v>
       </c>
       <c r="B582" t="s">
@@ -18344,7 +18337,7 @@
       </c>
     </row>
     <row r="583" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A583" s="2" t="s">
+      <c r="A583" t="s">
         <v>66</v>
       </c>
       <c r="B583" t="s">
@@ -18376,7 +18369,7 @@
       </c>
     </row>
     <row r="584" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A584" s="2" t="s">
+      <c r="A584" t="s">
         <v>66</v>
       </c>
       <c r="B584" t="s">
@@ -18408,7 +18401,7 @@
       </c>
     </row>
     <row r="585" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A585" s="2" t="s">
+      <c r="A585" t="s">
         <v>66</v>
       </c>
       <c r="B585" t="s">
@@ -18440,7 +18433,7 @@
       </c>
     </row>
     <row r="586" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A586" s="2" t="s">
+      <c r="A586" t="s">
         <v>66</v>
       </c>
       <c r="B586" t="s">
@@ -18472,7 +18465,7 @@
       </c>
     </row>
     <row r="587" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A587" s="2" t="s">
+      <c r="A587" t="s">
         <v>66</v>
       </c>
       <c r="B587" t="s">
@@ -18504,7 +18497,7 @@
       </c>
     </row>
     <row r="588" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A588" s="2" t="s">
+      <c r="A588" t="s">
         <v>66</v>
       </c>
       <c r="B588" t="s">
@@ -18536,7 +18529,7 @@
       </c>
     </row>
     <row r="589" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A589" s="2" t="s">
+      <c r="A589" t="s">
         <v>66</v>
       </c>
       <c r="B589" t="s">
@@ -18568,7 +18561,7 @@
       </c>
     </row>
     <row r="590" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A590" s="2" t="s">
+      <c r="A590" t="s">
         <v>66</v>
       </c>
       <c r="B590" t="s">
@@ -18600,7 +18593,7 @@
       </c>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A591" s="2" t="s">
+      <c r="A591" t="s">
         <v>66</v>
       </c>
       <c r="B591" t="s">
@@ -18632,7 +18625,7 @@
       </c>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A592" s="2" t="s">
+      <c r="A592" t="s">
         <v>66</v>
       </c>
       <c r="B592" t="s">
@@ -18664,7 +18657,7 @@
       </c>
     </row>
     <row r="593" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A593" s="2" t="s">
+      <c r="A593" t="s">
         <v>66</v>
       </c>
       <c r="B593" t="s">
@@ -18696,7 +18689,7 @@
       </c>
     </row>
     <row r="594" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A594" s="2" t="s">
+      <c r="A594" t="s">
         <v>66</v>
       </c>
       <c r="B594" t="s">
@@ -18728,7 +18721,7 @@
       </c>
     </row>
     <row r="595" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A595" s="2" t="s">
+      <c r="A595" t="s">
         <v>66</v>
       </c>
       <c r="B595" t="s">
@@ -18760,7 +18753,7 @@
       </c>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A597" s="2" t="s">
+      <c r="A597" t="s">
         <v>67</v>
       </c>
       <c r="B597" t="s">
@@ -18792,7 +18785,7 @@
       </c>
     </row>
     <row r="598" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A598" s="2" t="s">
+      <c r="A598" t="s">
         <v>67</v>
       </c>
       <c r="B598" t="s">
@@ -18824,7 +18817,7 @@
       </c>
     </row>
     <row r="599" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A599" s="2" t="s">
+      <c r="A599" t="s">
         <v>67</v>
       </c>
       <c r="B599" t="s">
@@ -18856,7 +18849,7 @@
       </c>
     </row>
     <row r="600" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A600" s="2" t="s">
+      <c r="A600" t="s">
         <v>67</v>
       </c>
       <c r="B600" t="s">
@@ -18888,7 +18881,7 @@
       </c>
     </row>
     <row r="601" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A601" s="2" t="s">
+      <c r="A601" t="s">
         <v>67</v>
       </c>
       <c r="B601" t="s">
@@ -18920,7 +18913,7 @@
       </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A602" s="2" t="s">
+      <c r="A602" t="s">
         <v>67</v>
       </c>
       <c r="B602" t="s">
@@ -18952,7 +18945,7 @@
       </c>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A603" s="2" t="s">
+      <c r="A603" t="s">
         <v>67</v>
       </c>
       <c r="B603" t="s">
@@ -18984,7 +18977,7 @@
       </c>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A604" s="2" t="s">
+      <c r="A604" t="s">
         <v>67</v>
       </c>
       <c r="B604" t="s">
@@ -19016,7 +19009,7 @@
       </c>
     </row>
     <row r="605" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A605" s="2" t="s">
+      <c r="A605" t="s">
         <v>67</v>
       </c>
       <c r="B605" t="s">
@@ -19048,7 +19041,7 @@
       </c>
     </row>
     <row r="606" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A606" s="2" t="s">
+      <c r="A606" t="s">
         <v>67</v>
       </c>
       <c r="B606" t="s">
@@ -19080,7 +19073,7 @@
       </c>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A607" s="2" t="s">
+      <c r="A607" t="s">
         <v>67</v>
       </c>
       <c r="B607" t="s">
@@ -19112,7 +19105,7 @@
       </c>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A608" s="2" t="s">
+      <c r="A608" t="s">
         <v>67</v>
       </c>
       <c r="B608" t="s">
@@ -19144,7 +19137,7 @@
       </c>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A609" s="2" t="s">
+      <c r="A609" t="s">
         <v>67</v>
       </c>
       <c r="B609" t="s">
@@ -19176,7 +19169,7 @@
       </c>
     </row>
     <row r="610" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A610" s="2" t="s">
+      <c r="A610" t="s">
         <v>67</v>
       </c>
       <c r="B610" t="s">
@@ -19208,7 +19201,7 @@
       </c>
     </row>
     <row r="611" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A611" s="2" t="s">
+      <c r="A611" t="s">
         <v>67</v>
       </c>
       <c r="B611" t="s">
@@ -19240,7 +19233,7 @@
       </c>
     </row>
     <row r="612" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A612" s="2" t="s">
+      <c r="A612" t="s">
         <v>67</v>
       </c>
       <c r="B612" t="s">
@@ -19272,7 +19265,7 @@
       </c>
     </row>
     <row r="614" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A614" s="2" t="s">
+      <c r="A614" t="s">
         <v>68</v>
       </c>
       <c r="B614" t="s">
@@ -19304,7 +19297,7 @@
       </c>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A615" s="2" t="s">
+      <c r="A615" t="s">
         <v>68</v>
       </c>
       <c r="B615" t="s">
@@ -19336,7 +19329,7 @@
       </c>
     </row>
     <row r="616" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A616" s="2" t="s">
+      <c r="A616" t="s">
         <v>68</v>
       </c>
       <c r="B616" t="s">
@@ -19368,7 +19361,7 @@
       </c>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A617" s="2" t="s">
+      <c r="A617" t="s">
         <v>68</v>
       </c>
       <c r="B617" t="s">
@@ -19400,7 +19393,7 @@
       </c>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A618" s="2" t="s">
+      <c r="A618" t="s">
         <v>68</v>
       </c>
       <c r="B618" t="s">
@@ -19432,7 +19425,7 @@
       </c>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A619" s="2" t="s">
+      <c r="A619" t="s">
         <v>68</v>
       </c>
       <c r="B619" t="s">
@@ -19464,7 +19457,7 @@
       </c>
     </row>
     <row r="620" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A620" s="2" t="s">
+      <c r="A620" t="s">
         <v>68</v>
       </c>
       <c r="B620" t="s">
@@ -19496,7 +19489,7 @@
       </c>
     </row>
     <row r="621" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A621" s="2" t="s">
+      <c r="A621" t="s">
         <v>68</v>
       </c>
       <c r="B621" t="s">
@@ -19528,7 +19521,7 @@
       </c>
     </row>
     <row r="622" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A622" s="2" t="s">
+      <c r="A622" t="s">
         <v>68</v>
       </c>
       <c r="B622" t="s">
@@ -19560,7 +19553,7 @@
       </c>
     </row>
     <row r="623" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A623" s="2" t="s">
+      <c r="A623" t="s">
         <v>68</v>
       </c>
       <c r="B623" t="s">
@@ -19592,7 +19585,7 @@
       </c>
     </row>
     <row r="624" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A624" s="2" t="s">
+      <c r="A624" t="s">
         <v>68</v>
       </c>
       <c r="B624" t="s">
@@ -19624,7 +19617,7 @@
       </c>
     </row>
     <row r="625" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A625" s="2" t="s">
+      <c r="A625" t="s">
         <v>68</v>
       </c>
       <c r="B625" t="s">
@@ -19656,7 +19649,7 @@
       </c>
     </row>
     <row r="626" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A626" s="2" t="s">
+      <c r="A626" t="s">
         <v>68</v>
       </c>
       <c r="B626" t="s">
@@ -19688,7 +19681,7 @@
       </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A627" s="2" t="s">
+      <c r="A627" t="s">
         <v>68</v>
       </c>
       <c r="B627" t="s">
@@ -19720,7 +19713,7 @@
       </c>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A628" s="2" t="s">
+      <c r="A628" t="s">
         <v>68</v>
       </c>
       <c r="B628" t="s">
@@ -19752,7 +19745,7 @@
       </c>
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A629" s="2" t="s">
+      <c r="A629" t="s">
         <v>68</v>
       </c>
       <c r="B629" t="s">
@@ -19784,7 +19777,7 @@
       </c>
     </row>
     <row r="631" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A631" s="2" t="s">
+      <c r="A631" t="s">
         <v>69</v>
       </c>
       <c r="B631" t="s">
@@ -19816,7 +19809,7 @@
       </c>
     </row>
     <row r="632" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A632" s="2" t="s">
+      <c r="A632" t="s">
         <v>69</v>
       </c>
       <c r="B632" t="s">
@@ -19848,7 +19841,7 @@
       </c>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A633" s="2" t="s">
+      <c r="A633" t="s">
         <v>69</v>
       </c>
       <c r="B633" t="s">
@@ -19880,7 +19873,7 @@
       </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A634" s="2" t="s">
+      <c r="A634" t="s">
         <v>69</v>
       </c>
       <c r="B634" t="s">
@@ -19912,7 +19905,7 @@
       </c>
     </row>
     <row r="635" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A635" s="2" t="s">
+      <c r="A635" t="s">
         <v>69</v>
       </c>
       <c r="B635" t="s">
@@ -19944,7 +19937,7 @@
       </c>
     </row>
     <row r="636" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A636" s="2" t="s">
+      <c r="A636" t="s">
         <v>69</v>
       </c>
       <c r="B636" t="s">
@@ -19976,7 +19969,7 @@
       </c>
     </row>
     <row r="637" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A637" s="2" t="s">
+      <c r="A637" t="s">
         <v>69</v>
       </c>
       <c r="B637" t="s">
@@ -20008,7 +20001,7 @@
       </c>
     </row>
     <row r="638" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A638" s="2" t="s">
+      <c r="A638" t="s">
         <v>69</v>
       </c>
       <c r="B638" t="s">
@@ -20040,7 +20033,7 @@
       </c>
     </row>
     <row r="639" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A639" s="2" t="s">
+      <c r="A639" t="s">
         <v>69</v>
       </c>
       <c r="B639" t="s">
@@ -20072,7 +20065,7 @@
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A640" s="2" t="s">
+      <c r="A640" t="s">
         <v>69</v>
       </c>
       <c r="B640" t="s">
@@ -20104,7 +20097,7 @@
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A641" s="2" t="s">
+      <c r="A641" t="s">
         <v>69</v>
       </c>
       <c r="B641" t="s">
@@ -20136,7 +20129,7 @@
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A642" s="2" t="s">
+      <c r="A642" t="s">
         <v>69</v>
       </c>
       <c r="B642" t="s">
@@ -20168,7 +20161,7 @@
       </c>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A643" s="2" t="s">
+      <c r="A643" t="s">
         <v>69</v>
       </c>
       <c r="B643" t="s">
@@ -20200,7 +20193,7 @@
       </c>
     </row>
     <row r="644" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A644" s="2" t="s">
+      <c r="A644" t="s">
         <v>69</v>
       </c>
       <c r="B644" t="s">
@@ -20232,7 +20225,7 @@
       </c>
     </row>
     <row r="645" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A645" s="2" t="s">
+      <c r="A645" t="s">
         <v>69</v>
       </c>
       <c r="B645" t="s">
@@ -20264,7 +20257,7 @@
       </c>
     </row>
     <row r="646" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A646" s="2" t="s">
+      <c r="A646" t="s">
         <v>69</v>
       </c>
       <c r="B646" t="s">
@@ -20296,7 +20289,7 @@
       </c>
     </row>
     <row r="648" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A648" s="2" t="s">
+      <c r="A648" t="s">
         <v>70</v>
       </c>
       <c r="B648" t="s">
@@ -20328,7 +20321,7 @@
       </c>
     </row>
     <row r="649" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A649" s="2" t="s">
+      <c r="A649" t="s">
         <v>70</v>
       </c>
       <c r="B649" t="s">
@@ -20360,7 +20353,7 @@
       </c>
     </row>
     <row r="650" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A650" s="2" t="s">
+      <c r="A650" t="s">
         <v>70</v>
       </c>
       <c r="B650" t="s">
@@ -20392,7 +20385,7 @@
       </c>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A651" s="2" t="s">
+      <c r="A651" t="s">
         <v>70</v>
       </c>
       <c r="B651" t="s">
@@ -20424,7 +20417,7 @@
       </c>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A652" s="2" t="s">
+      <c r="A652" t="s">
         <v>70</v>
       </c>
       <c r="B652" t="s">
@@ -20456,7 +20449,7 @@
       </c>
     </row>
     <row r="653" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A653" s="2" t="s">
+      <c r="A653" t="s">
         <v>70</v>
       </c>
       <c r="B653" t="s">
@@ -20488,7 +20481,7 @@
       </c>
     </row>
     <row r="654" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A654" s="2" t="s">
+      <c r="A654" t="s">
         <v>70</v>
       </c>
       <c r="B654" t="s">
@@ -20520,7 +20513,7 @@
       </c>
     </row>
     <row r="655" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A655" s="2" t="s">
+      <c r="A655" t="s">
         <v>70</v>
       </c>
       <c r="B655" t="s">
@@ -20552,7 +20545,7 @@
       </c>
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A656" s="2" t="s">
+      <c r="A656" t="s">
         <v>70</v>
       </c>
       <c r="B656" t="s">
@@ -20584,7 +20577,7 @@
       </c>
     </row>
     <row r="657" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A657" s="2" t="s">
+      <c r="A657" t="s">
         <v>70</v>
       </c>
       <c r="B657" t="s">
@@ -20616,7 +20609,7 @@
       </c>
     </row>
     <row r="658" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A658" s="2" t="s">
+      <c r="A658" t="s">
         <v>70</v>
       </c>
       <c r="B658" t="s">
@@ -20648,7 +20641,7 @@
       </c>
     </row>
     <row r="659" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A659" s="2" t="s">
+      <c r="A659" t="s">
         <v>70</v>
       </c>
       <c r="B659" t="s">
@@ -20680,7 +20673,7 @@
       </c>
     </row>
     <row r="660" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A660" s="2" t="s">
+      <c r="A660" t="s">
         <v>70</v>
       </c>
       <c r="B660" t="s">
@@ -20712,7 +20705,7 @@
       </c>
     </row>
     <row r="661" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A661" s="2" t="s">
+      <c r="A661" t="s">
         <v>70</v>
       </c>
       <c r="B661" t="s">
@@ -20744,7 +20737,7 @@
       </c>
     </row>
     <row r="662" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A662" s="2" t="s">
+      <c r="A662" t="s">
         <v>70</v>
       </c>
       <c r="B662" t="s">
@@ -20776,7 +20769,7 @@
       </c>
     </row>
     <row r="663" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A663" s="2" t="s">
+      <c r="A663" t="s">
         <v>70</v>
       </c>
       <c r="B663" t="s">
@@ -20808,7 +20801,7 @@
       </c>
     </row>
     <row r="665" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A665" s="2" t="s">
+      <c r="A665" t="s">
         <v>71</v>
       </c>
       <c r="B665" t="s">
@@ -20840,7 +20833,7 @@
       </c>
     </row>
     <row r="666" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A666" s="2" t="s">
+      <c r="A666" t="s">
         <v>71</v>
       </c>
       <c r="B666" t="s">
@@ -20872,7 +20865,7 @@
       </c>
     </row>
     <row r="667" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A667" s="2" t="s">
+      <c r="A667" t="s">
         <v>71</v>
       </c>
       <c r="B667" t="s">
@@ -20904,7 +20897,7 @@
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A668" s="2" t="s">
+      <c r="A668" t="s">
         <v>71</v>
       </c>
       <c r="B668" t="s">
@@ -20936,7 +20929,7 @@
       </c>
     </row>
     <row r="669" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A669" s="2" t="s">
+      <c r="A669" t="s">
         <v>71</v>
       </c>
       <c r="B669" t="s">
@@ -20968,7 +20961,7 @@
       </c>
     </row>
     <row r="670" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A670" s="2" t="s">
+      <c r="A670" t="s">
         <v>71</v>
       </c>
       <c r="B670" t="s">
@@ -21000,7 +20993,7 @@
       </c>
     </row>
     <row r="671" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A671" s="2" t="s">
+      <c r="A671" t="s">
         <v>71</v>
       </c>
       <c r="B671" t="s">
@@ -21032,7 +21025,7 @@
       </c>
     </row>
     <row r="672" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A672" s="2" t="s">
+      <c r="A672" t="s">
         <v>71</v>
       </c>
       <c r="B672" t="s">
@@ -21064,7 +21057,7 @@
       </c>
     </row>
     <row r="673" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A673" s="2" t="s">
+      <c r="A673" t="s">
         <v>71</v>
       </c>
       <c r="B673" t="s">
@@ -21096,7 +21089,7 @@
       </c>
     </row>
     <row r="674" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A674" s="2" t="s">
+      <c r="A674" t="s">
         <v>71</v>
       </c>
       <c r="B674" t="s">
@@ -21128,7 +21121,7 @@
       </c>
     </row>
     <row r="675" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A675" s="2" t="s">
+      <c r="A675" t="s">
         <v>71</v>
       </c>
       <c r="B675" t="s">
@@ -21160,7 +21153,7 @@
       </c>
     </row>
     <row r="676" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A676" s="2" t="s">
+      <c r="A676" t="s">
         <v>71</v>
       </c>
       <c r="B676" t="s">
@@ -21192,7 +21185,7 @@
       </c>
     </row>
     <row r="677" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A677" s="2" t="s">
+      <c r="A677" t="s">
         <v>71</v>
       </c>
       <c r="B677" t="s">
@@ -21224,7 +21217,7 @@
       </c>
     </row>
     <row r="678" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A678" s="2" t="s">
+      <c r="A678" t="s">
         <v>71</v>
       </c>
       <c r="B678" t="s">
@@ -21256,7 +21249,7 @@
       </c>
     </row>
     <row r="679" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A679" s="2" t="s">
+      <c r="A679" t="s">
         <v>71</v>
       </c>
       <c r="B679" t="s">
@@ -21288,7 +21281,7 @@
       </c>
     </row>
     <row r="680" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A680" s="2" t="s">
+      <c r="A680" t="s">
         <v>71</v>
       </c>
       <c r="B680" t="s">
@@ -21320,7 +21313,7 @@
       </c>
     </row>
     <row r="682" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A682" s="2" t="s">
+      <c r="A682" t="s">
         <v>72</v>
       </c>
       <c r="B682" t="s">
@@ -21352,7 +21345,7 @@
       </c>
     </row>
     <row r="683" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A683" s="2" t="s">
+      <c r="A683" t="s">
         <v>72</v>
       </c>
       <c r="B683" t="s">
@@ -21384,7 +21377,7 @@
       </c>
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A684" s="2" t="s">
+      <c r="A684" t="s">
         <v>72</v>
       </c>
       <c r="B684" t="s">
@@ -21416,7 +21409,7 @@
       </c>
     </row>
     <row r="685" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A685" s="2" t="s">
+      <c r="A685" t="s">
         <v>72</v>
       </c>
       <c r="B685" t="s">
@@ -21448,7 +21441,7 @@
       </c>
     </row>
     <row r="686" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A686" s="2" t="s">
+      <c r="A686" t="s">
         <v>72</v>
       </c>
       <c r="B686" t="s">
@@ -21480,7 +21473,7 @@
       </c>
     </row>
     <row r="687" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A687" s="2" t="s">
+      <c r="A687" t="s">
         <v>72</v>
       </c>
       <c r="B687" t="s">
@@ -21512,7 +21505,7 @@
       </c>
     </row>
     <row r="688" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A688" s="2" t="s">
+      <c r="A688" t="s">
         <v>72</v>
       </c>
       <c r="B688" t="s">
@@ -21544,7 +21537,7 @@
       </c>
     </row>
     <row r="689" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A689" s="2" t="s">
+      <c r="A689" t="s">
         <v>72</v>
       </c>
       <c r="B689" t="s">
@@ -21576,7 +21569,7 @@
       </c>
     </row>
     <row r="690" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A690" s="2" t="s">
+      <c r="A690" t="s">
         <v>72</v>
       </c>
       <c r="B690" t="s">
@@ -21608,7 +21601,7 @@
       </c>
     </row>
     <row r="691" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A691" s="2" t="s">
+      <c r="A691" t="s">
         <v>72</v>
       </c>
       <c r="B691" t="s">
@@ -21640,7 +21633,7 @@
       </c>
     </row>
     <row r="692" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A692" s="2" t="s">
+      <c r="A692" t="s">
         <v>72</v>
       </c>
       <c r="B692" t="s">
@@ -21672,7 +21665,7 @@
       </c>
     </row>
     <row r="693" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A693" s="2" t="s">
+      <c r="A693" t="s">
         <v>72</v>
       </c>
       <c r="B693" t="s">
@@ -21704,7 +21697,7 @@
       </c>
     </row>
     <row r="694" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A694" s="2" t="s">
+      <c r="A694" t="s">
         <v>72</v>
       </c>
       <c r="B694" t="s">
@@ -21736,7 +21729,7 @@
       </c>
     </row>
     <row r="695" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A695" s="2" t="s">
+      <c r="A695" t="s">
         <v>72</v>
       </c>
       <c r="B695" t="s">
@@ -21768,7 +21761,7 @@
       </c>
     </row>
     <row r="696" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A696" s="2" t="s">
+      <c r="A696" t="s">
         <v>72</v>
       </c>
       <c r="B696" t="s">
@@ -21800,7 +21793,7 @@
       </c>
     </row>
     <row r="697" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A697" s="2" t="s">
+      <c r="A697" t="s">
         <v>72</v>
       </c>
       <c r="B697" t="s">
@@ -21832,7 +21825,7 @@
       </c>
     </row>
     <row r="699" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A699" s="2" t="s">
+      <c r="A699" t="s">
         <v>73</v>
       </c>
       <c r="B699" t="s">
@@ -21864,7 +21857,7 @@
       </c>
     </row>
     <row r="700" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A700" s="2" t="s">
+      <c r="A700" t="s">
         <v>73</v>
       </c>
       <c r="B700" t="s">
@@ -21896,7 +21889,7 @@
       </c>
     </row>
     <row r="701" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A701" s="2" t="s">
+      <c r="A701" t="s">
         <v>73</v>
       </c>
       <c r="B701" t="s">
@@ -21928,7 +21921,7 @@
       </c>
     </row>
     <row r="702" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A702" s="2" t="s">
+      <c r="A702" t="s">
         <v>73</v>
       </c>
       <c r="B702" t="s">
@@ -21960,7 +21953,7 @@
       </c>
     </row>
     <row r="703" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A703" s="2" t="s">
+      <c r="A703" t="s">
         <v>73</v>
       </c>
       <c r="B703" t="s">
@@ -21992,7 +21985,7 @@
       </c>
     </row>
     <row r="704" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A704" s="2" t="s">
+      <c r="A704" t="s">
         <v>73</v>
       </c>
       <c r="B704" t="s">
@@ -22024,7 +22017,7 @@
       </c>
     </row>
     <row r="705" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A705" s="2" t="s">
+      <c r="A705" t="s">
         <v>73</v>
       </c>
       <c r="B705" t="s">
@@ -22056,7 +22049,7 @@
       </c>
     </row>
     <row r="706" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A706" s="2" t="s">
+      <c r="A706" t="s">
         <v>73</v>
       </c>
       <c r="B706" t="s">
@@ -22088,7 +22081,7 @@
       </c>
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A707" s="2" t="s">
+      <c r="A707" t="s">
         <v>73</v>
       </c>
       <c r="B707" t="s">
@@ -22120,7 +22113,7 @@
       </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A708" s="2" t="s">
+      <c r="A708" t="s">
         <v>73</v>
       </c>
       <c r="B708" t="s">
@@ -22152,7 +22145,7 @@
       </c>
     </row>
     <row r="709" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A709" s="2" t="s">
+      <c r="A709" t="s">
         <v>73</v>
       </c>
       <c r="B709" t="s">
@@ -22184,7 +22177,7 @@
       </c>
     </row>
     <row r="710" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A710" s="2" t="s">
+      <c r="A710" t="s">
         <v>73</v>
       </c>
       <c r="B710" t="s">
@@ -22216,7 +22209,7 @@
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A711" s="2" t="s">
+      <c r="A711" t="s">
         <v>73</v>
       </c>
       <c r="B711" t="s">
@@ -22248,7 +22241,7 @@
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A712" s="2" t="s">
+      <c r="A712" t="s">
         <v>73</v>
       </c>
       <c r="B712" t="s">
@@ -22280,7 +22273,7 @@
       </c>
     </row>
     <row r="713" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A713" s="2" t="s">
+      <c r="A713" t="s">
         <v>73</v>
       </c>
       <c r="B713" t="s">
@@ -22312,7 +22305,7 @@
       </c>
     </row>
     <row r="714" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A714" s="2" t="s">
+      <c r="A714" t="s">
         <v>73</v>
       </c>
       <c r="B714" t="s">
@@ -22344,7 +22337,7 @@
       </c>
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A716" s="2" t="s">
+      <c r="A716" t="s">
         <v>74</v>
       </c>
       <c r="B716" t="s">
@@ -22376,7 +22369,7 @@
       </c>
     </row>
     <row r="717" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A717" s="2" t="s">
+      <c r="A717" t="s">
         <v>74</v>
       </c>
       <c r="B717" t="s">
@@ -22408,7 +22401,7 @@
       </c>
     </row>
     <row r="718" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A718" s="2" t="s">
+      <c r="A718" t="s">
         <v>74</v>
       </c>
       <c r="B718" t="s">
@@ -22440,7 +22433,7 @@
       </c>
     </row>
     <row r="719" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A719" s="2" t="s">
+      <c r="A719" t="s">
         <v>74</v>
       </c>
       <c r="B719" t="s">
@@ -22472,7 +22465,7 @@
       </c>
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A720" s="2" t="s">
+      <c r="A720" t="s">
         <v>74</v>
       </c>
       <c r="B720" t="s">
@@ -22504,7 +22497,7 @@
       </c>
     </row>
     <row r="721" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A721" s="2" t="s">
+      <c r="A721" t="s">
         <v>74</v>
       </c>
       <c r="B721" t="s">
@@ -22536,7 +22529,7 @@
       </c>
     </row>
     <row r="722" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A722" s="2" t="s">
+      <c r="A722" t="s">
         <v>74</v>
       </c>
       <c r="B722" t="s">
@@ -22568,7 +22561,7 @@
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A723" s="2" t="s">
+      <c r="A723" t="s">
         <v>74</v>
       </c>
       <c r="B723" t="s">
@@ -22600,7 +22593,7 @@
       </c>
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A724" s="2" t="s">
+      <c r="A724" t="s">
         <v>74</v>
       </c>
       <c r="B724" t="s">
@@ -22632,7 +22625,7 @@
       </c>
     </row>
     <row r="725" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A725" s="2" t="s">
+      <c r="A725" t="s">
         <v>74</v>
       </c>
       <c r="B725" t="s">
@@ -22664,7 +22657,7 @@
       </c>
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A726" s="2" t="s">
+      <c r="A726" t="s">
         <v>74</v>
       </c>
       <c r="B726" t="s">
@@ -22696,7 +22689,7 @@
       </c>
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A727" s="2" t="s">
+      <c r="A727" t="s">
         <v>74</v>
       </c>
       <c r="B727" t="s">
@@ -22728,7 +22721,7 @@
       </c>
     </row>
     <row r="728" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A728" s="2" t="s">
+      <c r="A728" t="s">
         <v>74</v>
       </c>
       <c r="B728" t="s">
@@ -22760,7 +22753,7 @@
       </c>
     </row>
     <row r="729" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A729" s="2" t="s">
+      <c r="A729" t="s">
         <v>74</v>
       </c>
       <c r="B729" t="s">
@@ -22792,7 +22785,7 @@
       </c>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A730" s="2" t="s">
+      <c r="A730" t="s">
         <v>74</v>
       </c>
       <c r="B730" t="s">
@@ -22824,7 +22817,7 @@
       </c>
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A731" s="2" t="s">
+      <c r="A731" t="s">
         <v>74</v>
       </c>
       <c r="B731" t="s">
@@ -22856,7 +22849,7 @@
       </c>
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A733" s="2" t="s">
+      <c r="A733" t="s">
         <v>75</v>
       </c>
       <c r="B733" t="s">
@@ -22888,7 +22881,7 @@
       </c>
     </row>
     <row r="734" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A734" s="2" t="s">
+      <c r="A734" t="s">
         <v>75</v>
       </c>
       <c r="B734" t="s">
@@ -22920,7 +22913,7 @@
       </c>
     </row>
     <row r="735" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A735" s="2" t="s">
+      <c r="A735" t="s">
         <v>75</v>
       </c>
       <c r="B735" t="s">
@@ -22952,7 +22945,7 @@
       </c>
     </row>
     <row r="736" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A736" s="2" t="s">
+      <c r="A736" t="s">
         <v>75</v>
       </c>
       <c r="B736" t="s">
@@ -22984,7 +22977,7 @@
       </c>
     </row>
     <row r="737" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A737" s="2" t="s">
+      <c r="A737" t="s">
         <v>75</v>
       </c>
       <c r="B737" t="s">
@@ -23016,7 +23009,7 @@
       </c>
     </row>
     <row r="738" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A738" s="2" t="s">
+      <c r="A738" t="s">
         <v>75</v>
       </c>
       <c r="B738" t="s">
@@ -23048,7 +23041,7 @@
       </c>
     </row>
     <row r="739" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A739" s="2" t="s">
+      <c r="A739" t="s">
         <v>75</v>
       </c>
       <c r="B739" t="s">
@@ -23080,7 +23073,7 @@
       </c>
     </row>
     <row r="740" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A740" s="2" t="s">
+      <c r="A740" t="s">
         <v>75</v>
       </c>
       <c r="B740" t="s">
@@ -23112,7 +23105,7 @@
       </c>
     </row>
     <row r="741" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A741" s="2" t="s">
+      <c r="A741" t="s">
         <v>75</v>
       </c>
       <c r="B741" t="s">
@@ -23144,7 +23137,7 @@
       </c>
     </row>
     <row r="742" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A742" s="2" t="s">
+      <c r="A742" t="s">
         <v>75</v>
       </c>
       <c r="B742" t="s">
@@ -23176,7 +23169,7 @@
       </c>
     </row>
     <row r="743" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A743" s="2" t="s">
+      <c r="A743" t="s">
         <v>75</v>
       </c>
       <c r="B743" t="s">
@@ -23208,7 +23201,7 @@
       </c>
     </row>
     <row r="744" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A744" s="2" t="s">
+      <c r="A744" t="s">
         <v>75</v>
       </c>
       <c r="B744" t="s">
@@ -23240,7 +23233,7 @@
       </c>
     </row>
     <row r="745" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A745" s="2" t="s">
+      <c r="A745" t="s">
         <v>75</v>
       </c>
       <c r="B745" t="s">
@@ -23272,7 +23265,7 @@
       </c>
     </row>
     <row r="746" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A746" s="2" t="s">
+      <c r="A746" t="s">
         <v>75</v>
       </c>
       <c r="B746" t="s">
@@ -23304,7 +23297,7 @@
       </c>
     </row>
     <row r="747" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A747" s="2" t="s">
+      <c r="A747" t="s">
         <v>75</v>
       </c>
       <c r="B747" t="s">
@@ -23336,7 +23329,7 @@
       </c>
     </row>
     <row r="748" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A748" s="2" t="s">
+      <c r="A748" t="s">
         <v>75</v>
       </c>
       <c r="B748" t="s">
@@ -23368,7 +23361,7 @@
       </c>
     </row>
     <row r="750" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A750" s="2" t="s">
+      <c r="A750" t="s">
         <v>76</v>
       </c>
       <c r="B750" t="s">
@@ -23400,7 +23393,7 @@
       </c>
     </row>
     <row r="751" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A751" s="2" t="s">
+      <c r="A751" t="s">
         <v>76</v>
       </c>
       <c r="B751" t="s">
@@ -23432,7 +23425,7 @@
       </c>
     </row>
     <row r="752" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A752" s="2" t="s">
+      <c r="A752" t="s">
         <v>76</v>
       </c>
       <c r="B752" t="s">
@@ -23464,7 +23457,7 @@
       </c>
     </row>
     <row r="753" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A753" s="2" t="s">
+      <c r="A753" t="s">
         <v>76</v>
       </c>
       <c r="B753" t="s">
@@ -23496,7 +23489,7 @@
       </c>
     </row>
     <row r="754" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A754" s="2" t="s">
+      <c r="A754" t="s">
         <v>76</v>
       </c>
       <c r="B754" t="s">
@@ -23528,7 +23521,7 @@
       </c>
     </row>
     <row r="755" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A755" s="2" t="s">
+      <c r="A755" t="s">
         <v>76</v>
       </c>
       <c r="B755" t="s">
@@ -23560,7 +23553,7 @@
       </c>
     </row>
     <row r="756" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A756" s="2" t="s">
+      <c r="A756" t="s">
         <v>76</v>
       </c>
       <c r="B756" t="s">
@@ -23592,7 +23585,7 @@
       </c>
     </row>
     <row r="757" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A757" s="2" t="s">
+      <c r="A757" t="s">
         <v>76</v>
       </c>
       <c r="B757" t="s">
@@ -23624,7 +23617,7 @@
       </c>
     </row>
     <row r="758" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A758" s="2" t="s">
+      <c r="A758" t="s">
         <v>76</v>
       </c>
       <c r="B758" t="s">
@@ -23656,7 +23649,7 @@
       </c>
     </row>
     <row r="759" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A759" s="2" t="s">
+      <c r="A759" t="s">
         <v>76</v>
       </c>
       <c r="B759" t="s">
@@ -23688,7 +23681,7 @@
       </c>
     </row>
     <row r="760" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A760" s="2" t="s">
+      <c r="A760" t="s">
         <v>76</v>
       </c>
       <c r="B760" t="s">
@@ -23720,7 +23713,7 @@
       </c>
     </row>
     <row r="761" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A761" s="2" t="s">
+      <c r="A761" t="s">
         <v>76</v>
       </c>
       <c r="B761" t="s">
@@ -23752,7 +23745,7 @@
       </c>
     </row>
     <row r="762" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A762" s="2" t="s">
+      <c r="A762" t="s">
         <v>76</v>
       </c>
       <c r="B762" t="s">
@@ -23784,7 +23777,7 @@
       </c>
     </row>
     <row r="763" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A763" s="2" t="s">
+      <c r="A763" t="s">
         <v>76</v>
       </c>
       <c r="B763" t="s">
@@ -23816,7 +23809,7 @@
       </c>
     </row>
     <row r="764" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A764" s="2" t="s">
+      <c r="A764" t="s">
         <v>76</v>
       </c>
       <c r="B764" t="s">
@@ -23848,7 +23841,7 @@
       </c>
     </row>
     <row r="765" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A765" s="2" t="s">
+      <c r="A765" t="s">
         <v>76</v>
       </c>
       <c r="B765" t="s">
@@ -23880,7 +23873,7 @@
       </c>
     </row>
     <row r="767" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A767" s="2" t="s">
+      <c r="A767" t="s">
         <v>77</v>
       </c>
       <c r="B767" t="s">
@@ -23912,7 +23905,7 @@
       </c>
     </row>
     <row r="768" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A768" s="2" t="s">
+      <c r="A768" t="s">
         <v>77</v>
       </c>
       <c r="B768" t="s">
@@ -23944,7 +23937,7 @@
       </c>
     </row>
     <row r="769" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A769" s="2" t="s">
+      <c r="A769" t="s">
         <v>77</v>
       </c>
       <c r="B769" t="s">
@@ -23976,7 +23969,7 @@
       </c>
     </row>
     <row r="770" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A770" s="2" t="s">
+      <c r="A770" t="s">
         <v>77</v>
       </c>
       <c r="B770" t="s">
@@ -24008,7 +24001,7 @@
       </c>
     </row>
     <row r="771" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A771" s="2" t="s">
+      <c r="A771" t="s">
         <v>77</v>
       </c>
       <c r="B771" t="s">
@@ -24040,7 +24033,7 @@
       </c>
     </row>
     <row r="772" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A772" s="2" t="s">
+      <c r="A772" t="s">
         <v>77</v>
       </c>
       <c r="B772" t="s">
@@ -24072,7 +24065,7 @@
       </c>
     </row>
     <row r="773" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A773" s="2" t="s">
+      <c r="A773" t="s">
         <v>77</v>
       </c>
       <c r="B773" t="s">
@@ -24104,7 +24097,7 @@
       </c>
     </row>
     <row r="774" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A774" s="2" t="s">
+      <c r="A774" t="s">
         <v>77</v>
       </c>
       <c r="B774" t="s">
@@ -24136,7 +24129,7 @@
       </c>
     </row>
     <row r="775" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A775" s="2" t="s">
+      <c r="A775" t="s">
         <v>77</v>
       </c>
       <c r="B775" t="s">
@@ -24168,7 +24161,7 @@
       </c>
     </row>
     <row r="776" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A776" s="2" t="s">
+      <c r="A776" t="s">
         <v>77</v>
       </c>
       <c r="B776" t="s">
@@ -24200,7 +24193,7 @@
       </c>
     </row>
     <row r="777" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A777" s="2" t="s">
+      <c r="A777" t="s">
         <v>77</v>
       </c>
       <c r="B777" t="s">
@@ -24232,7 +24225,7 @@
       </c>
     </row>
     <row r="778" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A778" s="2" t="s">
+      <c r="A778" t="s">
         <v>77</v>
       </c>
       <c r="B778" t="s">
@@ -24264,7 +24257,7 @@
       </c>
     </row>
     <row r="779" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A779" s="2" t="s">
+      <c r="A779" t="s">
         <v>77</v>
       </c>
       <c r="B779" t="s">
@@ -24296,7 +24289,7 @@
       </c>
     </row>
     <row r="780" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A780" s="2" t="s">
+      <c r="A780" t="s">
         <v>77</v>
       </c>
       <c r="B780" t="s">
@@ -24328,7 +24321,7 @@
       </c>
     </row>
     <row r="781" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A781" s="2" t="s">
+      <c r="A781" t="s">
         <v>77</v>
       </c>
       <c r="B781" t="s">
@@ -24360,7 +24353,7 @@
       </c>
     </row>
     <row r="782" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A782" s="2" t="s">
+      <c r="A782" t="s">
         <v>77</v>
       </c>
       <c r="B782" t="s">
@@ -24392,7 +24385,7 @@
       </c>
     </row>
     <row r="784" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A784" s="2" t="s">
+      <c r="A784" t="s">
         <v>78</v>
       </c>
       <c r="B784" t="s">
@@ -24424,7 +24417,7 @@
       </c>
     </row>
     <row r="785" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A785" s="2" t="s">
+      <c r="A785" t="s">
         <v>78</v>
       </c>
       <c r="B785" t="s">
@@ -24456,7 +24449,7 @@
       </c>
     </row>
     <row r="786" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A786" s="2" t="s">
+      <c r="A786" t="s">
         <v>78</v>
       </c>
       <c r="B786" t="s">
@@ -24488,7 +24481,7 @@
       </c>
     </row>
     <row r="787" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A787" s="2" t="s">
+      <c r="A787" t="s">
         <v>78</v>
       </c>
       <c r="B787" t="s">
@@ -24520,7 +24513,7 @@
       </c>
     </row>
     <row r="788" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A788" s="2" t="s">
+      <c r="A788" t="s">
         <v>78</v>
       </c>
       <c r="B788" t="s">
@@ -24552,7 +24545,7 @@
       </c>
     </row>
     <row r="789" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A789" s="2" t="s">
+      <c r="A789" t="s">
         <v>78</v>
       </c>
       <c r="B789" t="s">
@@ -24584,7 +24577,7 @@
       </c>
     </row>
     <row r="790" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A790" s="2" t="s">
+      <c r="A790" t="s">
         <v>78</v>
       </c>
       <c r="B790" t="s">
@@ -24616,7 +24609,7 @@
       </c>
     </row>
     <row r="791" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A791" s="2" t="s">
+      <c r="A791" t="s">
         <v>78</v>
       </c>
       <c r="B791" t="s">
@@ -24648,7 +24641,7 @@
       </c>
     </row>
     <row r="792" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A792" s="2" t="s">
+      <c r="A792" t="s">
         <v>78</v>
       </c>
       <c r="B792" t="s">
@@ -24680,7 +24673,7 @@
       </c>
     </row>
     <row r="793" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A793" s="2" t="s">
+      <c r="A793" t="s">
         <v>78</v>
       </c>
       <c r="B793" t="s">
@@ -24712,7 +24705,7 @@
       </c>
     </row>
     <row r="794" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A794" s="2" t="s">
+      <c r="A794" t="s">
         <v>78</v>
       </c>
       <c r="B794" t="s">
@@ -24744,7 +24737,7 @@
       </c>
     </row>
     <row r="795" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A795" s="2" t="s">
+      <c r="A795" t="s">
         <v>78</v>
       </c>
       <c r="B795" t="s">
@@ -24776,7 +24769,7 @@
       </c>
     </row>
     <row r="796" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A796" s="2" t="s">
+      <c r="A796" t="s">
         <v>78</v>
       </c>
       <c r="B796" t="s">
@@ -24808,7 +24801,7 @@
       </c>
     </row>
     <row r="797" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A797" s="2" t="s">
+      <c r="A797" t="s">
         <v>78</v>
       </c>
       <c r="B797" t="s">
@@ -24840,7 +24833,7 @@
       </c>
     </row>
     <row r="798" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A798" s="2" t="s">
+      <c r="A798" t="s">
         <v>78</v>
       </c>
       <c r="B798" t="s">
@@ -24872,7 +24865,7 @@
       </c>
     </row>
     <row r="799" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A799" s="2" t="s">
+      <c r="A799" t="s">
         <v>78</v>
       </c>
       <c r="B799" t="s">
@@ -24904,7 +24897,7 @@
       </c>
     </row>
     <row r="801" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A801" s="2" t="s">
+      <c r="A801" t="s">
         <v>79</v>
       </c>
       <c r="B801" t="s">
@@ -24936,7 +24929,7 @@
       </c>
     </row>
     <row r="802" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A802" s="2" t="s">
+      <c r="A802" t="s">
         <v>79</v>
       </c>
       <c r="B802" t="s">
@@ -24968,7 +24961,7 @@
       </c>
     </row>
     <row r="803" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A803" s="2" t="s">
+      <c r="A803" t="s">
         <v>79</v>
       </c>
       <c r="B803" t="s">
@@ -25000,7 +24993,7 @@
       </c>
     </row>
     <row r="804" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A804" s="2" t="s">
+      <c r="A804" t="s">
         <v>79</v>
       </c>
       <c r="B804" t="s">
@@ -25032,7 +25025,7 @@
       </c>
     </row>
     <row r="805" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A805" s="2" t="s">
+      <c r="A805" t="s">
         <v>79</v>
       </c>
       <c r="B805" t="s">
@@ -25064,7 +25057,7 @@
       </c>
     </row>
     <row r="806" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A806" s="2" t="s">
+      <c r="A806" t="s">
         <v>79</v>
       </c>
       <c r="B806" t="s">
@@ -25096,7 +25089,7 @@
       </c>
     </row>
     <row r="807" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A807" s="2" t="s">
+      <c r="A807" t="s">
         <v>79</v>
       </c>
       <c r="B807" t="s">
@@ -25128,7 +25121,7 @@
       </c>
     </row>
     <row r="808" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A808" s="2" t="s">
+      <c r="A808" t="s">
         <v>79</v>
       </c>
       <c r="B808" t="s">
@@ -25160,7 +25153,7 @@
       </c>
     </row>
     <row r="809" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A809" s="2" t="s">
+      <c r="A809" t="s">
         <v>79</v>
       </c>
       <c r="B809" t="s">
@@ -25192,7 +25185,7 @@
       </c>
     </row>
     <row r="810" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A810" s="2" t="s">
+      <c r="A810" t="s">
         <v>79</v>
       </c>
       <c r="B810" t="s">
@@ -25224,7 +25217,7 @@
       </c>
     </row>
     <row r="811" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A811" s="2" t="s">
+      <c r="A811" t="s">
         <v>79</v>
       </c>
       <c r="B811" t="s">
@@ -25256,7 +25249,7 @@
       </c>
     </row>
     <row r="812" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A812" s="2" t="s">
+      <c r="A812" t="s">
         <v>79</v>
       </c>
       <c r="B812" t="s">
@@ -25288,7 +25281,7 @@
       </c>
     </row>
     <row r="813" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A813" s="2" t="s">
+      <c r="A813" t="s">
         <v>79</v>
       </c>
       <c r="B813" t="s">
@@ -25320,7 +25313,7 @@
       </c>
     </row>
     <row r="814" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A814" s="2" t="s">
+      <c r="A814" t="s">
         <v>79</v>
       </c>
       <c r="B814" t="s">
@@ -25352,7 +25345,7 @@
       </c>
     </row>
     <row r="815" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A815" s="2" t="s">
+      <c r="A815" t="s">
         <v>79</v>
       </c>
       <c r="B815" t="s">
@@ -25384,7 +25377,7 @@
       </c>
     </row>
     <row r="816" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A816" s="2" t="s">
+      <c r="A816" t="s">
         <v>79</v>
       </c>
       <c r="B816" t="s">

</xml_diff>

<commit_message>
May 16 Misc Changes
</commit_message>
<xml_diff>
--- a/PXD020586/sdrf.xlsx
+++ b/PXD020586/sdrf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Payne Lab\TMT\TMT_QC\PXD020586\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB7531B-DD3C-400F-BE58-3D57F692336B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD88E175-63DA-4741-BD64-97959C3A8B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B0FF2B6B-E326-450E-82DA-7E4299F0AAC8}"/>
   </bookViews>
@@ -414,7 +414,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,12 +427,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,12 +449,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0AE791-64B6-4DAB-A49D-D63DB87399C3}">
   <dimension ref="A1:J1428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1340" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1354" sqref="D1354"/>
     </sheetView>
   </sheetViews>
@@ -15688,7 +15681,7 @@
       </c>
     </row>
     <row r="495" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A495" s="2" t="s">
+      <c r="A495" t="s">
         <v>61</v>
       </c>
       <c r="B495" t="s">
@@ -15720,7 +15713,7 @@
       </c>
     </row>
     <row r="496" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A496" s="2" t="s">
+      <c r="A496" t="s">
         <v>61</v>
       </c>
       <c r="B496" t="s">
@@ -15752,7 +15745,7 @@
       </c>
     </row>
     <row r="497" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A497" s="2" t="s">
+      <c r="A497" t="s">
         <v>61</v>
       </c>
       <c r="B497" t="s">
@@ -15784,7 +15777,7 @@
       </c>
     </row>
     <row r="498" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A498" s="2" t="s">
+      <c r="A498" t="s">
         <v>61</v>
       </c>
       <c r="B498" t="s">
@@ -15816,7 +15809,7 @@
       </c>
     </row>
     <row r="499" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A499" s="2" t="s">
+      <c r="A499" t="s">
         <v>61</v>
       </c>
       <c r="B499" t="s">
@@ -15848,7 +15841,7 @@
       </c>
     </row>
     <row r="500" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A500" s="2" t="s">
+      <c r="A500" t="s">
         <v>61</v>
       </c>
       <c r="B500" t="s">
@@ -15880,7 +15873,7 @@
       </c>
     </row>
     <row r="501" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A501" s="2" t="s">
+      <c r="A501" t="s">
         <v>61</v>
       </c>
       <c r="B501" t="s">
@@ -15912,7 +15905,7 @@
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A502" s="2" t="s">
+      <c r="A502" t="s">
         <v>61</v>
       </c>
       <c r="B502" t="s">
@@ -15944,7 +15937,7 @@
       </c>
     </row>
     <row r="503" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A503" s="2" t="s">
+      <c r="A503" t="s">
         <v>61</v>
       </c>
       <c r="B503" t="s">
@@ -15976,7 +15969,7 @@
       </c>
     </row>
     <row r="504" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A504" s="2" t="s">
+      <c r="A504" t="s">
         <v>61</v>
       </c>
       <c r="B504" t="s">
@@ -16008,7 +16001,7 @@
       </c>
     </row>
     <row r="505" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A505" s="2" t="s">
+      <c r="A505" t="s">
         <v>61</v>
       </c>
       <c r="B505" t="s">
@@ -16040,7 +16033,7 @@
       </c>
     </row>
     <row r="506" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A506" s="2" t="s">
+      <c r="A506" t="s">
         <v>61</v>
       </c>
       <c r="B506" t="s">
@@ -16072,7 +16065,7 @@
       </c>
     </row>
     <row r="507" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A507" s="2" t="s">
+      <c r="A507" t="s">
         <v>61</v>
       </c>
       <c r="B507" t="s">
@@ -16104,7 +16097,7 @@
       </c>
     </row>
     <row r="508" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A508" s="2" t="s">
+      <c r="A508" t="s">
         <v>61</v>
       </c>
       <c r="B508" t="s">
@@ -16136,7 +16129,7 @@
       </c>
     </row>
     <row r="509" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A509" s="2" t="s">
+      <c r="A509" t="s">
         <v>61</v>
       </c>
       <c r="B509" t="s">
@@ -16168,7 +16161,7 @@
       </c>
     </row>
     <row r="510" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A510" s="2" t="s">
+      <c r="A510" t="s">
         <v>61</v>
       </c>
       <c r="B510" t="s">
@@ -16200,7 +16193,7 @@
       </c>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A512" s="2" t="s">
+      <c r="A512" t="s">
         <v>62</v>
       </c>
       <c r="B512" t="s">
@@ -16232,7 +16225,7 @@
       </c>
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A513" s="2" t="s">
+      <c r="A513" t="s">
         <v>62</v>
       </c>
       <c r="B513" t="s">
@@ -16264,7 +16257,7 @@
       </c>
     </row>
     <row r="514" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A514" s="2" t="s">
+      <c r="A514" t="s">
         <v>62</v>
       </c>
       <c r="B514" t="s">
@@ -16296,7 +16289,7 @@
       </c>
     </row>
     <row r="515" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A515" s="2" t="s">
+      <c r="A515" t="s">
         <v>62</v>
       </c>
       <c r="B515" t="s">
@@ -16328,7 +16321,7 @@
       </c>
     </row>
     <row r="516" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A516" s="2" t="s">
+      <c r="A516" t="s">
         <v>62</v>
       </c>
       <c r="B516" t="s">
@@ -16360,7 +16353,7 @@
       </c>
     </row>
     <row r="517" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A517" s="2" t="s">
+      <c r="A517" t="s">
         <v>62</v>
       </c>
       <c r="B517" t="s">
@@ -16392,7 +16385,7 @@
       </c>
     </row>
     <row r="518" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A518" s="2" t="s">
+      <c r="A518" t="s">
         <v>62</v>
       </c>
       <c r="B518" t="s">
@@ -16424,7 +16417,7 @@
       </c>
     </row>
     <row r="519" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A519" s="2" t="s">
+      <c r="A519" t="s">
         <v>62</v>
       </c>
       <c r="B519" t="s">
@@ -16456,7 +16449,7 @@
       </c>
     </row>
     <row r="520" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A520" s="2" t="s">
+      <c r="A520" t="s">
         <v>62</v>
       </c>
       <c r="B520" t="s">
@@ -16488,7 +16481,7 @@
       </c>
     </row>
     <row r="521" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A521" s="2" t="s">
+      <c r="A521" t="s">
         <v>62</v>
       </c>
       <c r="B521" t="s">
@@ -16520,7 +16513,7 @@
       </c>
     </row>
     <row r="522" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A522" s="2" t="s">
+      <c r="A522" t="s">
         <v>62</v>
       </c>
       <c r="B522" t="s">
@@ -16552,7 +16545,7 @@
       </c>
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A523" s="2" t="s">
+      <c r="A523" t="s">
         <v>62</v>
       </c>
       <c r="B523" t="s">
@@ -16584,7 +16577,7 @@
       </c>
     </row>
     <row r="524" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A524" s="2" t="s">
+      <c r="A524" t="s">
         <v>62</v>
       </c>
       <c r="B524" t="s">
@@ -16616,7 +16609,7 @@
       </c>
     </row>
     <row r="525" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A525" s="2" t="s">
+      <c r="A525" t="s">
         <v>62</v>
       </c>
       <c r="B525" t="s">
@@ -16648,7 +16641,7 @@
       </c>
     </row>
     <row r="526" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A526" s="2" t="s">
+      <c r="A526" t="s">
         <v>62</v>
       </c>
       <c r="B526" t="s">
@@ -16680,7 +16673,7 @@
       </c>
     </row>
     <row r="527" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A527" s="2" t="s">
+      <c r="A527" t="s">
         <v>62</v>
       </c>
       <c r="B527" t="s">
@@ -16712,7 +16705,7 @@
       </c>
     </row>
     <row r="529" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A529" s="2" t="s">
+      <c r="A529" t="s">
         <v>63</v>
       </c>
       <c r="B529" t="s">
@@ -16744,7 +16737,7 @@
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A530" s="2" t="s">
+      <c r="A530" t="s">
         <v>63</v>
       </c>
       <c r="B530" t="s">
@@ -16776,7 +16769,7 @@
       </c>
     </row>
     <row r="531" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A531" s="2" t="s">
+      <c r="A531" t="s">
         <v>63</v>
       </c>
       <c r="B531" t="s">
@@ -16808,7 +16801,7 @@
       </c>
     </row>
     <row r="532" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A532" s="2" t="s">
+      <c r="A532" t="s">
         <v>63</v>
       </c>
       <c r="B532" t="s">
@@ -16840,7 +16833,7 @@
       </c>
     </row>
     <row r="533" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A533" s="2" t="s">
+      <c r="A533" t="s">
         <v>63</v>
       </c>
       <c r="B533" t="s">
@@ -16872,7 +16865,7 @@
       </c>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A534" s="2" t="s">
+      <c r="A534" t="s">
         <v>63</v>
       </c>
       <c r="B534" t="s">
@@ -16904,7 +16897,7 @@
       </c>
     </row>
     <row r="535" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A535" s="2" t="s">
+      <c r="A535" t="s">
         <v>63</v>
       </c>
       <c r="B535" t="s">
@@ -16936,7 +16929,7 @@
       </c>
     </row>
     <row r="536" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A536" s="2" t="s">
+      <c r="A536" t="s">
         <v>63</v>
       </c>
       <c r="B536" t="s">
@@ -16968,7 +16961,7 @@
       </c>
     </row>
     <row r="537" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A537" s="2" t="s">
+      <c r="A537" t="s">
         <v>63</v>
       </c>
       <c r="B537" t="s">
@@ -17000,7 +16993,7 @@
       </c>
     </row>
     <row r="538" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A538" s="2" t="s">
+      <c r="A538" t="s">
         <v>63</v>
       </c>
       <c r="B538" t="s">
@@ -17032,7 +17025,7 @@
       </c>
     </row>
     <row r="539" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A539" s="2" t="s">
+      <c r="A539" t="s">
         <v>63</v>
       </c>
       <c r="B539" t="s">
@@ -17064,7 +17057,7 @@
       </c>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A540" s="2" t="s">
+      <c r="A540" t="s">
         <v>63</v>
       </c>
       <c r="B540" t="s">
@@ -17096,7 +17089,7 @@
       </c>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A541" s="2" t="s">
+      <c r="A541" t="s">
         <v>63</v>
       </c>
       <c r="B541" t="s">
@@ -17128,7 +17121,7 @@
       </c>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A542" s="2" t="s">
+      <c r="A542" t="s">
         <v>63</v>
       </c>
       <c r="B542" t="s">
@@ -17160,7 +17153,7 @@
       </c>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A543" s="2" t="s">
+      <c r="A543" t="s">
         <v>63</v>
       </c>
       <c r="B543" t="s">
@@ -17192,7 +17185,7 @@
       </c>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A544" s="2" t="s">
+      <c r="A544" t="s">
         <v>63</v>
       </c>
       <c r="B544" t="s">
@@ -17224,7 +17217,7 @@
       </c>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A546" s="2" t="s">
+      <c r="A546" t="s">
         <v>64</v>
       </c>
       <c r="B546" t="s">
@@ -17256,7 +17249,7 @@
       </c>
     </row>
     <row r="547" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A547" s="2" t="s">
+      <c r="A547" t="s">
         <v>64</v>
       </c>
       <c r="B547" t="s">
@@ -17288,7 +17281,7 @@
       </c>
     </row>
     <row r="548" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A548" s="2" t="s">
+      <c r="A548" t="s">
         <v>64</v>
       </c>
       <c r="B548" t="s">
@@ -17320,7 +17313,7 @@
       </c>
     </row>
     <row r="549" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A549" s="2" t="s">
+      <c r="A549" t="s">
         <v>64</v>
       </c>
       <c r="B549" t="s">
@@ -17352,7 +17345,7 @@
       </c>
     </row>
     <row r="550" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A550" s="2" t="s">
+      <c r="A550" t="s">
         <v>64</v>
       </c>
       <c r="B550" t="s">
@@ -17384,7 +17377,7 @@
       </c>
     </row>
     <row r="551" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A551" s="2" t="s">
+      <c r="A551" t="s">
         <v>64</v>
       </c>
       <c r="B551" t="s">
@@ -17416,7 +17409,7 @@
       </c>
     </row>
     <row r="552" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A552" s="2" t="s">
+      <c r="A552" t="s">
         <v>64</v>
       </c>
       <c r="B552" t="s">
@@ -17448,7 +17441,7 @@
       </c>
     </row>
     <row r="553" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A553" s="2" t="s">
+      <c r="A553" t="s">
         <v>64</v>
       </c>
       <c r="B553" t="s">
@@ -17480,7 +17473,7 @@
       </c>
     </row>
     <row r="554" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A554" s="2" t="s">
+      <c r="A554" t="s">
         <v>64</v>
       </c>
       <c r="B554" t="s">
@@ -17512,7 +17505,7 @@
       </c>
     </row>
     <row r="555" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A555" s="2" t="s">
+      <c r="A555" t="s">
         <v>64</v>
       </c>
       <c r="B555" t="s">
@@ -17544,7 +17537,7 @@
       </c>
     </row>
     <row r="556" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A556" s="2" t="s">
+      <c r="A556" t="s">
         <v>64</v>
       </c>
       <c r="B556" t="s">
@@ -17576,7 +17569,7 @@
       </c>
     </row>
     <row r="557" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A557" s="2" t="s">
+      <c r="A557" t="s">
         <v>64</v>
       </c>
       <c r="B557" t="s">
@@ -17608,7 +17601,7 @@
       </c>
     </row>
     <row r="558" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A558" s="2" t="s">
+      <c r="A558" t="s">
         <v>64</v>
       </c>
       <c r="B558" t="s">
@@ -17640,7 +17633,7 @@
       </c>
     </row>
     <row r="559" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A559" s="2" t="s">
+      <c r="A559" t="s">
         <v>64</v>
       </c>
       <c r="B559" t="s">
@@ -17672,7 +17665,7 @@
       </c>
     </row>
     <row r="560" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A560" s="2" t="s">
+      <c r="A560" t="s">
         <v>64</v>
       </c>
       <c r="B560" t="s">
@@ -17704,7 +17697,7 @@
       </c>
     </row>
     <row r="561" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A561" s="2" t="s">
+      <c r="A561" t="s">
         <v>64</v>
       </c>
       <c r="B561" t="s">
@@ -17736,7 +17729,7 @@
       </c>
     </row>
     <row r="563" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A563" s="2" t="s">
+      <c r="A563" t="s">
         <v>65</v>
       </c>
       <c r="B563" t="s">
@@ -17768,7 +17761,7 @@
       </c>
     </row>
     <row r="564" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A564" s="2" t="s">
+      <c r="A564" t="s">
         <v>65</v>
       </c>
       <c r="B564" t="s">
@@ -17800,7 +17793,7 @@
       </c>
     </row>
     <row r="565" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A565" s="2" t="s">
+      <c r="A565" t="s">
         <v>65</v>
       </c>
       <c r="B565" t="s">
@@ -17832,7 +17825,7 @@
       </c>
     </row>
     <row r="566" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A566" s="2" t="s">
+      <c r="A566" t="s">
         <v>65</v>
       </c>
       <c r="B566" t="s">
@@ -17864,7 +17857,7 @@
       </c>
     </row>
     <row r="567" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A567" s="2" t="s">
+      <c r="A567" t="s">
         <v>65</v>
       </c>
       <c r="B567" t="s">
@@ -17896,7 +17889,7 @@
       </c>
     </row>
     <row r="568" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A568" s="2" t="s">
+      <c r="A568" t="s">
         <v>65</v>
       </c>
       <c r="B568" t="s">
@@ -17928,7 +17921,7 @@
       </c>
     </row>
     <row r="569" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A569" s="2" t="s">
+      <c r="A569" t="s">
         <v>65</v>
       </c>
       <c r="B569" t="s">
@@ -17960,7 +17953,7 @@
       </c>
     </row>
     <row r="570" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A570" s="2" t="s">
+      <c r="A570" t="s">
         <v>65</v>
       </c>
       <c r="B570" t="s">
@@ -17992,7 +17985,7 @@
       </c>
     </row>
     <row r="571" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A571" s="2" t="s">
+      <c r="A571" t="s">
         <v>65</v>
       </c>
       <c r="B571" t="s">
@@ -18024,7 +18017,7 @@
       </c>
     </row>
     <row r="572" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A572" s="2" t="s">
+      <c r="A572" t="s">
         <v>65</v>
       </c>
       <c r="B572" t="s">
@@ -18056,7 +18049,7 @@
       </c>
     </row>
     <row r="573" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A573" s="2" t="s">
+      <c r="A573" t="s">
         <v>65</v>
       </c>
       <c r="B573" t="s">
@@ -18088,7 +18081,7 @@
       </c>
     </row>
     <row r="574" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A574" s="2" t="s">
+      <c r="A574" t="s">
         <v>65</v>
       </c>
       <c r="B574" t="s">
@@ -18120,7 +18113,7 @@
       </c>
     </row>
     <row r="575" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A575" s="2" t="s">
+      <c r="A575" t="s">
         <v>65</v>
       </c>
       <c r="B575" t="s">
@@ -18152,7 +18145,7 @@
       </c>
     </row>
     <row r="576" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A576" s="2" t="s">
+      <c r="A576" t="s">
         <v>65</v>
       </c>
       <c r="B576" t="s">
@@ -18184,7 +18177,7 @@
       </c>
     </row>
     <row r="577" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A577" s="2" t="s">
+      <c r="A577" t="s">
         <v>65</v>
       </c>
       <c r="B577" t="s">
@@ -18216,7 +18209,7 @@
       </c>
     </row>
     <row r="578" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A578" s="2" t="s">
+      <c r="A578" t="s">
         <v>65</v>
       </c>
       <c r="B578" t="s">
@@ -18248,7 +18241,7 @@
       </c>
     </row>
     <row r="580" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A580" s="2" t="s">
+      <c r="A580" t="s">
         <v>66</v>
       </c>
       <c r="B580" t="s">
@@ -18280,7 +18273,7 @@
       </c>
     </row>
     <row r="581" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A581" s="2" t="s">
+      <c r="A581" t="s">
         <v>66</v>
       </c>
       <c r="B581" t="s">
@@ -18312,7 +18305,7 @@
       </c>
     </row>
     <row r="582" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A582" s="2" t="s">
+      <c r="A582" t="s">
         <v>66</v>
       </c>
       <c r="B582" t="s">
@@ -18344,7 +18337,7 @@
       </c>
     </row>
     <row r="583" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A583" s="2" t="s">
+      <c r="A583" t="s">
         <v>66</v>
       </c>
       <c r="B583" t="s">
@@ -18376,7 +18369,7 @@
       </c>
     </row>
     <row r="584" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A584" s="2" t="s">
+      <c r="A584" t="s">
         <v>66</v>
       </c>
       <c r="B584" t="s">
@@ -18408,7 +18401,7 @@
       </c>
     </row>
     <row r="585" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A585" s="2" t="s">
+      <c r="A585" t="s">
         <v>66</v>
       </c>
       <c r="B585" t="s">
@@ -18440,7 +18433,7 @@
       </c>
     </row>
     <row r="586" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A586" s="2" t="s">
+      <c r="A586" t="s">
         <v>66</v>
       </c>
       <c r="B586" t="s">
@@ -18472,7 +18465,7 @@
       </c>
     </row>
     <row r="587" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A587" s="2" t="s">
+      <c r="A587" t="s">
         <v>66</v>
       </c>
       <c r="B587" t="s">
@@ -18504,7 +18497,7 @@
       </c>
     </row>
     <row r="588" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A588" s="2" t="s">
+      <c r="A588" t="s">
         <v>66</v>
       </c>
       <c r="B588" t="s">
@@ -18536,7 +18529,7 @@
       </c>
     </row>
     <row r="589" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A589" s="2" t="s">
+      <c r="A589" t="s">
         <v>66</v>
       </c>
       <c r="B589" t="s">
@@ -18568,7 +18561,7 @@
       </c>
     </row>
     <row r="590" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A590" s="2" t="s">
+      <c r="A590" t="s">
         <v>66</v>
       </c>
       <c r="B590" t="s">
@@ -18600,7 +18593,7 @@
       </c>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A591" s="2" t="s">
+      <c r="A591" t="s">
         <v>66</v>
       </c>
       <c r="B591" t="s">
@@ -18632,7 +18625,7 @@
       </c>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A592" s="2" t="s">
+      <c r="A592" t="s">
         <v>66</v>
       </c>
       <c r="B592" t="s">
@@ -18664,7 +18657,7 @@
       </c>
     </row>
     <row r="593" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A593" s="2" t="s">
+      <c r="A593" t="s">
         <v>66</v>
       </c>
       <c r="B593" t="s">
@@ -18696,7 +18689,7 @@
       </c>
     </row>
     <row r="594" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A594" s="2" t="s">
+      <c r="A594" t="s">
         <v>66</v>
       </c>
       <c r="B594" t="s">
@@ -18728,7 +18721,7 @@
       </c>
     </row>
     <row r="595" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A595" s="2" t="s">
+      <c r="A595" t="s">
         <v>66</v>
       </c>
       <c r="B595" t="s">
@@ -18760,7 +18753,7 @@
       </c>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A597" s="2" t="s">
+      <c r="A597" t="s">
         <v>67</v>
       </c>
       <c r="B597" t="s">
@@ -18792,7 +18785,7 @@
       </c>
     </row>
     <row r="598" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A598" s="2" t="s">
+      <c r="A598" t="s">
         <v>67</v>
       </c>
       <c r="B598" t="s">
@@ -18824,7 +18817,7 @@
       </c>
     </row>
     <row r="599" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A599" s="2" t="s">
+      <c r="A599" t="s">
         <v>67</v>
       </c>
       <c r="B599" t="s">
@@ -18856,7 +18849,7 @@
       </c>
     </row>
     <row r="600" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A600" s="2" t="s">
+      <c r="A600" t="s">
         <v>67</v>
       </c>
       <c r="B600" t="s">
@@ -18888,7 +18881,7 @@
       </c>
     </row>
     <row r="601" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A601" s="2" t="s">
+      <c r="A601" t="s">
         <v>67</v>
       </c>
       <c r="B601" t="s">
@@ -18920,7 +18913,7 @@
       </c>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A602" s="2" t="s">
+      <c r="A602" t="s">
         <v>67</v>
       </c>
       <c r="B602" t="s">
@@ -18952,7 +18945,7 @@
       </c>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A603" s="2" t="s">
+      <c r="A603" t="s">
         <v>67</v>
       </c>
       <c r="B603" t="s">
@@ -18984,7 +18977,7 @@
       </c>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A604" s="2" t="s">
+      <c r="A604" t="s">
         <v>67</v>
       </c>
       <c r="B604" t="s">
@@ -19016,7 +19009,7 @@
       </c>
     </row>
     <row r="605" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A605" s="2" t="s">
+      <c r="A605" t="s">
         <v>67</v>
       </c>
       <c r="B605" t="s">
@@ -19048,7 +19041,7 @@
       </c>
     </row>
     <row r="606" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A606" s="2" t="s">
+      <c r="A606" t="s">
         <v>67</v>
       </c>
       <c r="B606" t="s">
@@ -19080,7 +19073,7 @@
       </c>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A607" s="2" t="s">
+      <c r="A607" t="s">
         <v>67</v>
       </c>
       <c r="B607" t="s">
@@ -19112,7 +19105,7 @@
       </c>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A608" s="2" t="s">
+      <c r="A608" t="s">
         <v>67</v>
       </c>
       <c r="B608" t="s">
@@ -19144,7 +19137,7 @@
       </c>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A609" s="2" t="s">
+      <c r="A609" t="s">
         <v>67</v>
       </c>
       <c r="B609" t="s">
@@ -19176,7 +19169,7 @@
       </c>
     </row>
     <row r="610" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A610" s="2" t="s">
+      <c r="A610" t="s">
         <v>67</v>
       </c>
       <c r="B610" t="s">
@@ -19208,7 +19201,7 @@
       </c>
     </row>
     <row r="611" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A611" s="2" t="s">
+      <c r="A611" t="s">
         <v>67</v>
       </c>
       <c r="B611" t="s">
@@ -19240,7 +19233,7 @@
       </c>
     </row>
     <row r="612" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A612" s="2" t="s">
+      <c r="A612" t="s">
         <v>67</v>
       </c>
       <c r="B612" t="s">
@@ -19272,7 +19265,7 @@
       </c>
     </row>
     <row r="614" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A614" s="2" t="s">
+      <c r="A614" t="s">
         <v>68</v>
       </c>
       <c r="B614" t="s">
@@ -19304,7 +19297,7 @@
       </c>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A615" s="2" t="s">
+      <c r="A615" t="s">
         <v>68</v>
       </c>
       <c r="B615" t="s">
@@ -19336,7 +19329,7 @@
       </c>
     </row>
     <row r="616" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A616" s="2" t="s">
+      <c r="A616" t="s">
         <v>68</v>
       </c>
       <c r="B616" t="s">
@@ -19368,7 +19361,7 @@
       </c>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A617" s="2" t="s">
+      <c r="A617" t="s">
         <v>68</v>
       </c>
       <c r="B617" t="s">
@@ -19400,7 +19393,7 @@
       </c>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A618" s="2" t="s">
+      <c r="A618" t="s">
         <v>68</v>
       </c>
       <c r="B618" t="s">
@@ -19432,7 +19425,7 @@
       </c>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A619" s="2" t="s">
+      <c r="A619" t="s">
         <v>68</v>
       </c>
       <c r="B619" t="s">
@@ -19464,7 +19457,7 @@
       </c>
     </row>
     <row r="620" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A620" s="2" t="s">
+      <c r="A620" t="s">
         <v>68</v>
       </c>
       <c r="B620" t="s">
@@ -19496,7 +19489,7 @@
       </c>
     </row>
     <row r="621" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A621" s="2" t="s">
+      <c r="A621" t="s">
         <v>68</v>
       </c>
       <c r="B621" t="s">
@@ -19528,7 +19521,7 @@
       </c>
     </row>
     <row r="622" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A622" s="2" t="s">
+      <c r="A622" t="s">
         <v>68</v>
       </c>
       <c r="B622" t="s">
@@ -19560,7 +19553,7 @@
       </c>
     </row>
     <row r="623" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A623" s="2" t="s">
+      <c r="A623" t="s">
         <v>68</v>
       </c>
       <c r="B623" t="s">
@@ -19592,7 +19585,7 @@
       </c>
     </row>
     <row r="624" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A624" s="2" t="s">
+      <c r="A624" t="s">
         <v>68</v>
       </c>
       <c r="B624" t="s">
@@ -19624,7 +19617,7 @@
       </c>
     </row>
     <row r="625" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A625" s="2" t="s">
+      <c r="A625" t="s">
         <v>68</v>
       </c>
       <c r="B625" t="s">
@@ -19656,7 +19649,7 @@
       </c>
     </row>
     <row r="626" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A626" s="2" t="s">
+      <c r="A626" t="s">
         <v>68</v>
       </c>
       <c r="B626" t="s">
@@ -19688,7 +19681,7 @@
       </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A627" s="2" t="s">
+      <c r="A627" t="s">
         <v>68</v>
       </c>
       <c r="B627" t="s">
@@ -19720,7 +19713,7 @@
       </c>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A628" s="2" t="s">
+      <c r="A628" t="s">
         <v>68</v>
       </c>
       <c r="B628" t="s">
@@ -19752,7 +19745,7 @@
       </c>
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A629" s="2" t="s">
+      <c r="A629" t="s">
         <v>68</v>
       </c>
       <c r="B629" t="s">
@@ -19784,7 +19777,7 @@
       </c>
     </row>
     <row r="631" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A631" s="2" t="s">
+      <c r="A631" t="s">
         <v>69</v>
       </c>
       <c r="B631" t="s">
@@ -19816,7 +19809,7 @@
       </c>
     </row>
     <row r="632" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A632" s="2" t="s">
+      <c r="A632" t="s">
         <v>69</v>
       </c>
       <c r="B632" t="s">
@@ -19848,7 +19841,7 @@
       </c>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A633" s="2" t="s">
+      <c r="A633" t="s">
         <v>69</v>
       </c>
       <c r="B633" t="s">
@@ -19880,7 +19873,7 @@
       </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A634" s="2" t="s">
+      <c r="A634" t="s">
         <v>69</v>
       </c>
       <c r="B634" t="s">
@@ -19912,7 +19905,7 @@
       </c>
     </row>
     <row r="635" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A635" s="2" t="s">
+      <c r="A635" t="s">
         <v>69</v>
       </c>
       <c r="B635" t="s">
@@ -19944,7 +19937,7 @@
       </c>
     </row>
     <row r="636" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A636" s="2" t="s">
+      <c r="A636" t="s">
         <v>69</v>
       </c>
       <c r="B636" t="s">
@@ -19976,7 +19969,7 @@
       </c>
     </row>
     <row r="637" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A637" s="2" t="s">
+      <c r="A637" t="s">
         <v>69</v>
       </c>
       <c r="B637" t="s">
@@ -20008,7 +20001,7 @@
       </c>
     </row>
     <row r="638" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A638" s="2" t="s">
+      <c r="A638" t="s">
         <v>69</v>
       </c>
       <c r="B638" t="s">
@@ -20040,7 +20033,7 @@
       </c>
     </row>
     <row r="639" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A639" s="2" t="s">
+      <c r="A639" t="s">
         <v>69</v>
       </c>
       <c r="B639" t="s">
@@ -20072,7 +20065,7 @@
       </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A640" s="2" t="s">
+      <c r="A640" t="s">
         <v>69</v>
       </c>
       <c r="B640" t="s">
@@ -20104,7 +20097,7 @@
       </c>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A641" s="2" t="s">
+      <c r="A641" t="s">
         <v>69</v>
       </c>
       <c r="B641" t="s">
@@ -20136,7 +20129,7 @@
       </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A642" s="2" t="s">
+      <c r="A642" t="s">
         <v>69</v>
       </c>
       <c r="B642" t="s">
@@ -20168,7 +20161,7 @@
       </c>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A643" s="2" t="s">
+      <c r="A643" t="s">
         <v>69</v>
       </c>
       <c r="B643" t="s">
@@ -20200,7 +20193,7 @@
       </c>
     </row>
     <row r="644" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A644" s="2" t="s">
+      <c r="A644" t="s">
         <v>69</v>
       </c>
       <c r="B644" t="s">
@@ -20232,7 +20225,7 @@
       </c>
     </row>
     <row r="645" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A645" s="2" t="s">
+      <c r="A645" t="s">
         <v>69</v>
       </c>
       <c r="B645" t="s">
@@ -20264,7 +20257,7 @@
       </c>
     </row>
     <row r="646" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A646" s="2" t="s">
+      <c r="A646" t="s">
         <v>69</v>
       </c>
       <c r="B646" t="s">
@@ -20296,7 +20289,7 @@
       </c>
     </row>
     <row r="648" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A648" s="2" t="s">
+      <c r="A648" t="s">
         <v>70</v>
       </c>
       <c r="B648" t="s">
@@ -20328,7 +20321,7 @@
       </c>
     </row>
     <row r="649" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A649" s="2" t="s">
+      <c r="A649" t="s">
         <v>70</v>
       </c>
       <c r="B649" t="s">
@@ -20360,7 +20353,7 @@
       </c>
     </row>
     <row r="650" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A650" s="2" t="s">
+      <c r="A650" t="s">
         <v>70</v>
       </c>
       <c r="B650" t="s">
@@ -20392,7 +20385,7 @@
       </c>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A651" s="2" t="s">
+      <c r="A651" t="s">
         <v>70</v>
       </c>
       <c r="B651" t="s">
@@ -20424,7 +20417,7 @@
       </c>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A652" s="2" t="s">
+      <c r="A652" t="s">
         <v>70</v>
       </c>
       <c r="B652" t="s">
@@ -20456,7 +20449,7 @@
       </c>
     </row>
     <row r="653" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A653" s="2" t="s">
+      <c r="A653" t="s">
         <v>70</v>
       </c>
       <c r="B653" t="s">
@@ -20488,7 +20481,7 @@
       </c>
     </row>
     <row r="654" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A654" s="2" t="s">
+      <c r="A654" t="s">
         <v>70</v>
       </c>
       <c r="B654" t="s">
@@ -20520,7 +20513,7 @@
       </c>
     </row>
     <row r="655" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A655" s="2" t="s">
+      <c r="A655" t="s">
         <v>70</v>
       </c>
       <c r="B655" t="s">
@@ -20552,7 +20545,7 @@
       </c>
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A656" s="2" t="s">
+      <c r="A656" t="s">
         <v>70</v>
       </c>
       <c r="B656" t="s">
@@ -20584,7 +20577,7 @@
       </c>
     </row>
     <row r="657" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A657" s="2" t="s">
+      <c r="A657" t="s">
         <v>70</v>
       </c>
       <c r="B657" t="s">
@@ -20616,7 +20609,7 @@
       </c>
     </row>
     <row r="658" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A658" s="2" t="s">
+      <c r="A658" t="s">
         <v>70</v>
       </c>
       <c r="B658" t="s">
@@ -20648,7 +20641,7 @@
       </c>
     </row>
     <row r="659" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A659" s="2" t="s">
+      <c r="A659" t="s">
         <v>70</v>
       </c>
       <c r="B659" t="s">
@@ -20680,7 +20673,7 @@
       </c>
     </row>
     <row r="660" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A660" s="2" t="s">
+      <c r="A660" t="s">
         <v>70</v>
       </c>
       <c r="B660" t="s">
@@ -20712,7 +20705,7 @@
       </c>
     </row>
     <row r="661" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A661" s="2" t="s">
+      <c r="A661" t="s">
         <v>70</v>
       </c>
       <c r="B661" t="s">
@@ -20744,7 +20737,7 @@
       </c>
     </row>
     <row r="662" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A662" s="2" t="s">
+      <c r="A662" t="s">
         <v>70</v>
       </c>
       <c r="B662" t="s">
@@ -20776,7 +20769,7 @@
       </c>
     </row>
     <row r="663" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A663" s="2" t="s">
+      <c r="A663" t="s">
         <v>70</v>
       </c>
       <c r="B663" t="s">
@@ -20808,7 +20801,7 @@
       </c>
     </row>
     <row r="665" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A665" s="2" t="s">
+      <c r="A665" t="s">
         <v>71</v>
       </c>
       <c r="B665" t="s">
@@ -20840,7 +20833,7 @@
       </c>
     </row>
     <row r="666" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A666" s="2" t="s">
+      <c r="A666" t="s">
         <v>71</v>
       </c>
       <c r="B666" t="s">
@@ -20872,7 +20865,7 @@
       </c>
     </row>
     <row r="667" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A667" s="2" t="s">
+      <c r="A667" t="s">
         <v>71</v>
       </c>
       <c r="B667" t="s">
@@ -20904,7 +20897,7 @@
       </c>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A668" s="2" t="s">
+      <c r="A668" t="s">
         <v>71</v>
       </c>
       <c r="B668" t="s">
@@ -20936,7 +20929,7 @@
       </c>
     </row>
     <row r="669" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A669" s="2" t="s">
+      <c r="A669" t="s">
         <v>71</v>
       </c>
       <c r="B669" t="s">
@@ -20968,7 +20961,7 @@
       </c>
     </row>
     <row r="670" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A670" s="2" t="s">
+      <c r="A670" t="s">
         <v>71</v>
       </c>
       <c r="B670" t="s">
@@ -21000,7 +20993,7 @@
       </c>
     </row>
     <row r="671" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A671" s="2" t="s">
+      <c r="A671" t="s">
         <v>71</v>
       </c>
       <c r="B671" t="s">
@@ -21032,7 +21025,7 @@
       </c>
     </row>
     <row r="672" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A672" s="2" t="s">
+      <c r="A672" t="s">
         <v>71</v>
       </c>
       <c r="B672" t="s">
@@ -21064,7 +21057,7 @@
       </c>
     </row>
     <row r="673" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A673" s="2" t="s">
+      <c r="A673" t="s">
         <v>71</v>
       </c>
       <c r="B673" t="s">
@@ -21096,7 +21089,7 @@
       </c>
     </row>
     <row r="674" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A674" s="2" t="s">
+      <c r="A674" t="s">
         <v>71</v>
       </c>
       <c r="B674" t="s">
@@ -21128,7 +21121,7 @@
       </c>
     </row>
     <row r="675" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A675" s="2" t="s">
+      <c r="A675" t="s">
         <v>71</v>
       </c>
       <c r="B675" t="s">
@@ -21160,7 +21153,7 @@
       </c>
     </row>
     <row r="676" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A676" s="2" t="s">
+      <c r="A676" t="s">
         <v>71</v>
       </c>
       <c r="B676" t="s">
@@ -21192,7 +21185,7 @@
       </c>
     </row>
     <row r="677" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A677" s="2" t="s">
+      <c r="A677" t="s">
         <v>71</v>
       </c>
       <c r="B677" t="s">
@@ -21224,7 +21217,7 @@
       </c>
     </row>
     <row r="678" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A678" s="2" t="s">
+      <c r="A678" t="s">
         <v>71</v>
       </c>
       <c r="B678" t="s">
@@ -21256,7 +21249,7 @@
       </c>
     </row>
     <row r="679" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A679" s="2" t="s">
+      <c r="A679" t="s">
         <v>71</v>
       </c>
       <c r="B679" t="s">
@@ -21288,7 +21281,7 @@
       </c>
     </row>
     <row r="680" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A680" s="2" t="s">
+      <c r="A680" t="s">
         <v>71</v>
       </c>
       <c r="B680" t="s">
@@ -21320,7 +21313,7 @@
       </c>
     </row>
     <row r="682" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A682" s="2" t="s">
+      <c r="A682" t="s">
         <v>72</v>
       </c>
       <c r="B682" t="s">
@@ -21352,7 +21345,7 @@
       </c>
     </row>
     <row r="683" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A683" s="2" t="s">
+      <c r="A683" t="s">
         <v>72</v>
       </c>
       <c r="B683" t="s">
@@ -21384,7 +21377,7 @@
       </c>
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A684" s="2" t="s">
+      <c r="A684" t="s">
         <v>72</v>
       </c>
       <c r="B684" t="s">
@@ -21416,7 +21409,7 @@
       </c>
     </row>
     <row r="685" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A685" s="2" t="s">
+      <c r="A685" t="s">
         <v>72</v>
       </c>
       <c r="B685" t="s">
@@ -21448,7 +21441,7 @@
       </c>
     </row>
     <row r="686" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A686" s="2" t="s">
+      <c r="A686" t="s">
         <v>72</v>
       </c>
       <c r="B686" t="s">
@@ -21480,7 +21473,7 @@
       </c>
     </row>
     <row r="687" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A687" s="2" t="s">
+      <c r="A687" t="s">
         <v>72</v>
       </c>
       <c r="B687" t="s">
@@ -21512,7 +21505,7 @@
       </c>
     </row>
     <row r="688" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A688" s="2" t="s">
+      <c r="A688" t="s">
         <v>72</v>
       </c>
       <c r="B688" t="s">
@@ -21544,7 +21537,7 @@
       </c>
     </row>
     <row r="689" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A689" s="2" t="s">
+      <c r="A689" t="s">
         <v>72</v>
       </c>
       <c r="B689" t="s">
@@ -21576,7 +21569,7 @@
       </c>
     </row>
     <row r="690" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A690" s="2" t="s">
+      <c r="A690" t="s">
         <v>72</v>
       </c>
       <c r="B690" t="s">
@@ -21608,7 +21601,7 @@
       </c>
     </row>
     <row r="691" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A691" s="2" t="s">
+      <c r="A691" t="s">
         <v>72</v>
       </c>
       <c r="B691" t="s">
@@ -21640,7 +21633,7 @@
       </c>
     </row>
     <row r="692" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A692" s="2" t="s">
+      <c r="A692" t="s">
         <v>72</v>
       </c>
       <c r="B692" t="s">
@@ -21672,7 +21665,7 @@
       </c>
     </row>
     <row r="693" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A693" s="2" t="s">
+      <c r="A693" t="s">
         <v>72</v>
       </c>
       <c r="B693" t="s">
@@ -21704,7 +21697,7 @@
       </c>
     </row>
     <row r="694" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A694" s="2" t="s">
+      <c r="A694" t="s">
         <v>72</v>
       </c>
       <c r="B694" t="s">
@@ -21736,7 +21729,7 @@
       </c>
     </row>
     <row r="695" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A695" s="2" t="s">
+      <c r="A695" t="s">
         <v>72</v>
       </c>
       <c r="B695" t="s">
@@ -21768,7 +21761,7 @@
       </c>
     </row>
     <row r="696" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A696" s="2" t="s">
+      <c r="A696" t="s">
         <v>72</v>
       </c>
       <c r="B696" t="s">
@@ -21800,7 +21793,7 @@
       </c>
     </row>
     <row r="697" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A697" s="2" t="s">
+      <c r="A697" t="s">
         <v>72</v>
       </c>
       <c r="B697" t="s">
@@ -21832,7 +21825,7 @@
       </c>
     </row>
     <row r="699" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A699" s="2" t="s">
+      <c r="A699" t="s">
         <v>73</v>
       </c>
       <c r="B699" t="s">
@@ -21864,7 +21857,7 @@
       </c>
     </row>
     <row r="700" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A700" s="2" t="s">
+      <c r="A700" t="s">
         <v>73</v>
       </c>
       <c r="B700" t="s">
@@ -21896,7 +21889,7 @@
       </c>
     </row>
     <row r="701" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A701" s="2" t="s">
+      <c r="A701" t="s">
         <v>73</v>
       </c>
       <c r="B701" t="s">
@@ -21928,7 +21921,7 @@
       </c>
     </row>
     <row r="702" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A702" s="2" t="s">
+      <c r="A702" t="s">
         <v>73</v>
       </c>
       <c r="B702" t="s">
@@ -21960,7 +21953,7 @@
       </c>
     </row>
     <row r="703" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A703" s="2" t="s">
+      <c r="A703" t="s">
         <v>73</v>
       </c>
       <c r="B703" t="s">
@@ -21992,7 +21985,7 @@
       </c>
     </row>
     <row r="704" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A704" s="2" t="s">
+      <c r="A704" t="s">
         <v>73</v>
       </c>
       <c r="B704" t="s">
@@ -22024,7 +22017,7 @@
       </c>
     </row>
     <row r="705" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A705" s="2" t="s">
+      <c r="A705" t="s">
         <v>73</v>
       </c>
       <c r="B705" t="s">
@@ -22056,7 +22049,7 @@
       </c>
     </row>
     <row r="706" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A706" s="2" t="s">
+      <c r="A706" t="s">
         <v>73</v>
       </c>
       <c r="B706" t="s">
@@ -22088,7 +22081,7 @@
       </c>
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A707" s="2" t="s">
+      <c r="A707" t="s">
         <v>73</v>
       </c>
       <c r="B707" t="s">
@@ -22120,7 +22113,7 @@
       </c>
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A708" s="2" t="s">
+      <c r="A708" t="s">
         <v>73</v>
       </c>
       <c r="B708" t="s">
@@ -22152,7 +22145,7 @@
       </c>
     </row>
     <row r="709" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A709" s="2" t="s">
+      <c r="A709" t="s">
         <v>73</v>
       </c>
       <c r="B709" t="s">
@@ -22184,7 +22177,7 @@
       </c>
     </row>
     <row r="710" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A710" s="2" t="s">
+      <c r="A710" t="s">
         <v>73</v>
       </c>
       <c r="B710" t="s">
@@ -22216,7 +22209,7 @@
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A711" s="2" t="s">
+      <c r="A711" t="s">
         <v>73</v>
       </c>
       <c r="B711" t="s">
@@ -22248,7 +22241,7 @@
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A712" s="2" t="s">
+      <c r="A712" t="s">
         <v>73</v>
       </c>
       <c r="B712" t="s">
@@ -22280,7 +22273,7 @@
       </c>
     </row>
     <row r="713" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A713" s="2" t="s">
+      <c r="A713" t="s">
         <v>73</v>
       </c>
       <c r="B713" t="s">
@@ -22312,7 +22305,7 @@
       </c>
     </row>
     <row r="714" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A714" s="2" t="s">
+      <c r="A714" t="s">
         <v>73</v>
       </c>
       <c r="B714" t="s">
@@ -22344,7 +22337,7 @@
       </c>
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A716" s="2" t="s">
+      <c r="A716" t="s">
         <v>74</v>
       </c>
       <c r="B716" t="s">
@@ -22376,7 +22369,7 @@
       </c>
     </row>
     <row r="717" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A717" s="2" t="s">
+      <c r="A717" t="s">
         <v>74</v>
       </c>
       <c r="B717" t="s">
@@ -22408,7 +22401,7 @@
       </c>
     </row>
     <row r="718" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A718" s="2" t="s">
+      <c r="A718" t="s">
         <v>74</v>
       </c>
       <c r="B718" t="s">
@@ -22440,7 +22433,7 @@
       </c>
     </row>
     <row r="719" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A719" s="2" t="s">
+      <c r="A719" t="s">
         <v>74</v>
       </c>
       <c r="B719" t="s">
@@ -22472,7 +22465,7 @@
       </c>
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A720" s="2" t="s">
+      <c r="A720" t="s">
         <v>74</v>
       </c>
       <c r="B720" t="s">
@@ -22504,7 +22497,7 @@
       </c>
     </row>
     <row r="721" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A721" s="2" t="s">
+      <c r="A721" t="s">
         <v>74</v>
       </c>
       <c r="B721" t="s">
@@ -22536,7 +22529,7 @@
       </c>
     </row>
     <row r="722" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A722" s="2" t="s">
+      <c r="A722" t="s">
         <v>74</v>
       </c>
       <c r="B722" t="s">
@@ -22568,7 +22561,7 @@
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A723" s="2" t="s">
+      <c r="A723" t="s">
         <v>74</v>
       </c>
       <c r="B723" t="s">
@@ -22600,7 +22593,7 @@
       </c>
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A724" s="2" t="s">
+      <c r="A724" t="s">
         <v>74</v>
       </c>
       <c r="B724" t="s">
@@ -22632,7 +22625,7 @@
       </c>
     </row>
     <row r="725" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A725" s="2" t="s">
+      <c r="A725" t="s">
         <v>74</v>
       </c>
       <c r="B725" t="s">
@@ -22664,7 +22657,7 @@
       </c>
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A726" s="2" t="s">
+      <c r="A726" t="s">
         <v>74</v>
       </c>
       <c r="B726" t="s">
@@ -22696,7 +22689,7 @@
       </c>
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A727" s="2" t="s">
+      <c r="A727" t="s">
         <v>74</v>
       </c>
       <c r="B727" t="s">
@@ -22728,7 +22721,7 @@
       </c>
     </row>
     <row r="728" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A728" s="2" t="s">
+      <c r="A728" t="s">
         <v>74</v>
       </c>
       <c r="B728" t="s">
@@ -22760,7 +22753,7 @@
       </c>
     </row>
     <row r="729" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A729" s="2" t="s">
+      <c r="A729" t="s">
         <v>74</v>
       </c>
       <c r="B729" t="s">
@@ -22792,7 +22785,7 @@
       </c>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A730" s="2" t="s">
+      <c r="A730" t="s">
         <v>74</v>
       </c>
       <c r="B730" t="s">
@@ -22824,7 +22817,7 @@
       </c>
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A731" s="2" t="s">
+      <c r="A731" t="s">
         <v>74</v>
       </c>
       <c r="B731" t="s">
@@ -22856,7 +22849,7 @@
       </c>
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A733" s="2" t="s">
+      <c r="A733" t="s">
         <v>75</v>
       </c>
       <c r="B733" t="s">
@@ -22888,7 +22881,7 @@
       </c>
     </row>
     <row r="734" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A734" s="2" t="s">
+      <c r="A734" t="s">
         <v>75</v>
       </c>
       <c r="B734" t="s">
@@ -22920,7 +22913,7 @@
       </c>
     </row>
     <row r="735" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A735" s="2" t="s">
+      <c r="A735" t="s">
         <v>75</v>
       </c>
       <c r="B735" t="s">
@@ -22952,7 +22945,7 @@
       </c>
     </row>
     <row r="736" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A736" s="2" t="s">
+      <c r="A736" t="s">
         <v>75</v>
       </c>
       <c r="B736" t="s">
@@ -22984,7 +22977,7 @@
       </c>
     </row>
     <row r="737" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A737" s="2" t="s">
+      <c r="A737" t="s">
         <v>75</v>
       </c>
       <c r="B737" t="s">
@@ -23016,7 +23009,7 @@
       </c>
     </row>
     <row r="738" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A738" s="2" t="s">
+      <c r="A738" t="s">
         <v>75</v>
       </c>
       <c r="B738" t="s">
@@ -23048,7 +23041,7 @@
       </c>
     </row>
     <row r="739" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A739" s="2" t="s">
+      <c r="A739" t="s">
         <v>75</v>
       </c>
       <c r="B739" t="s">
@@ -23080,7 +23073,7 @@
       </c>
     </row>
     <row r="740" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A740" s="2" t="s">
+      <c r="A740" t="s">
         <v>75</v>
       </c>
       <c r="B740" t="s">
@@ -23112,7 +23105,7 @@
       </c>
     </row>
     <row r="741" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A741" s="2" t="s">
+      <c r="A741" t="s">
         <v>75</v>
       </c>
       <c r="B741" t="s">
@@ -23144,7 +23137,7 @@
       </c>
     </row>
     <row r="742" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A742" s="2" t="s">
+      <c r="A742" t="s">
         <v>75</v>
       </c>
       <c r="B742" t="s">
@@ -23176,7 +23169,7 @@
       </c>
     </row>
     <row r="743" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A743" s="2" t="s">
+      <c r="A743" t="s">
         <v>75</v>
       </c>
       <c r="B743" t="s">
@@ -23208,7 +23201,7 @@
       </c>
     </row>
     <row r="744" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A744" s="2" t="s">
+      <c r="A744" t="s">
         <v>75</v>
       </c>
       <c r="B744" t="s">
@@ -23240,7 +23233,7 @@
       </c>
     </row>
     <row r="745" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A745" s="2" t="s">
+      <c r="A745" t="s">
         <v>75</v>
       </c>
       <c r="B745" t="s">
@@ -23272,7 +23265,7 @@
       </c>
     </row>
     <row r="746" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A746" s="2" t="s">
+      <c r="A746" t="s">
         <v>75</v>
       </c>
       <c r="B746" t="s">
@@ -23304,7 +23297,7 @@
       </c>
     </row>
     <row r="747" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A747" s="2" t="s">
+      <c r="A747" t="s">
         <v>75</v>
       </c>
       <c r="B747" t="s">
@@ -23336,7 +23329,7 @@
       </c>
     </row>
     <row r="748" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A748" s="2" t="s">
+      <c r="A748" t="s">
         <v>75</v>
       </c>
       <c r="B748" t="s">
@@ -23368,7 +23361,7 @@
       </c>
     </row>
     <row r="750" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A750" s="2" t="s">
+      <c r="A750" t="s">
         <v>76</v>
       </c>
       <c r="B750" t="s">
@@ -23400,7 +23393,7 @@
       </c>
     </row>
     <row r="751" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A751" s="2" t="s">
+      <c r="A751" t="s">
         <v>76</v>
       </c>
       <c r="B751" t="s">
@@ -23432,7 +23425,7 @@
       </c>
     </row>
     <row r="752" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A752" s="2" t="s">
+      <c r="A752" t="s">
         <v>76</v>
       </c>
       <c r="B752" t="s">
@@ -23464,7 +23457,7 @@
       </c>
     </row>
     <row r="753" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A753" s="2" t="s">
+      <c r="A753" t="s">
         <v>76</v>
       </c>
       <c r="B753" t="s">
@@ -23496,7 +23489,7 @@
       </c>
     </row>
     <row r="754" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A754" s="2" t="s">
+      <c r="A754" t="s">
         <v>76</v>
       </c>
       <c r="B754" t="s">
@@ -23528,7 +23521,7 @@
       </c>
     </row>
     <row r="755" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A755" s="2" t="s">
+      <c r="A755" t="s">
         <v>76</v>
       </c>
       <c r="B755" t="s">
@@ -23560,7 +23553,7 @@
       </c>
     </row>
     <row r="756" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A756" s="2" t="s">
+      <c r="A756" t="s">
         <v>76</v>
       </c>
       <c r="B756" t="s">
@@ -23592,7 +23585,7 @@
       </c>
     </row>
     <row r="757" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A757" s="2" t="s">
+      <c r="A757" t="s">
         <v>76</v>
       </c>
       <c r="B757" t="s">
@@ -23624,7 +23617,7 @@
       </c>
     </row>
     <row r="758" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A758" s="2" t="s">
+      <c r="A758" t="s">
         <v>76</v>
       </c>
       <c r="B758" t="s">
@@ -23656,7 +23649,7 @@
       </c>
     </row>
     <row r="759" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A759" s="2" t="s">
+      <c r="A759" t="s">
         <v>76</v>
       </c>
       <c r="B759" t="s">
@@ -23688,7 +23681,7 @@
       </c>
     </row>
     <row r="760" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A760" s="2" t="s">
+      <c r="A760" t="s">
         <v>76</v>
       </c>
       <c r="B760" t="s">
@@ -23720,7 +23713,7 @@
       </c>
     </row>
     <row r="761" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A761" s="2" t="s">
+      <c r="A761" t="s">
         <v>76</v>
       </c>
       <c r="B761" t="s">
@@ -23752,7 +23745,7 @@
       </c>
     </row>
     <row r="762" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A762" s="2" t="s">
+      <c r="A762" t="s">
         <v>76</v>
       </c>
       <c r="B762" t="s">
@@ -23784,7 +23777,7 @@
       </c>
     </row>
     <row r="763" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A763" s="2" t="s">
+      <c r="A763" t="s">
         <v>76</v>
       </c>
       <c r="B763" t="s">
@@ -23816,7 +23809,7 @@
       </c>
     </row>
     <row r="764" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A764" s="2" t="s">
+      <c r="A764" t="s">
         <v>76</v>
       </c>
       <c r="B764" t="s">
@@ -23848,7 +23841,7 @@
       </c>
     </row>
     <row r="765" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A765" s="2" t="s">
+      <c r="A765" t="s">
         <v>76</v>
       </c>
       <c r="B765" t="s">
@@ -23880,7 +23873,7 @@
       </c>
     </row>
     <row r="767" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A767" s="2" t="s">
+      <c r="A767" t="s">
         <v>77</v>
       </c>
       <c r="B767" t="s">
@@ -23912,7 +23905,7 @@
       </c>
     </row>
     <row r="768" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A768" s="2" t="s">
+      <c r="A768" t="s">
         <v>77</v>
       </c>
       <c r="B768" t="s">
@@ -23944,7 +23937,7 @@
       </c>
     </row>
     <row r="769" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A769" s="2" t="s">
+      <c r="A769" t="s">
         <v>77</v>
       </c>
       <c r="B769" t="s">
@@ -23976,7 +23969,7 @@
       </c>
     </row>
     <row r="770" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A770" s="2" t="s">
+      <c r="A770" t="s">
         <v>77</v>
       </c>
       <c r="B770" t="s">
@@ -24008,7 +24001,7 @@
       </c>
     </row>
     <row r="771" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A771" s="2" t="s">
+      <c r="A771" t="s">
         <v>77</v>
       </c>
       <c r="B771" t="s">
@@ -24040,7 +24033,7 @@
       </c>
     </row>
     <row r="772" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A772" s="2" t="s">
+      <c r="A772" t="s">
         <v>77</v>
       </c>
       <c r="B772" t="s">
@@ -24072,7 +24065,7 @@
       </c>
     </row>
     <row r="773" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A773" s="2" t="s">
+      <c r="A773" t="s">
         <v>77</v>
       </c>
       <c r="B773" t="s">
@@ -24104,7 +24097,7 @@
       </c>
     </row>
     <row r="774" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A774" s="2" t="s">
+      <c r="A774" t="s">
         <v>77</v>
       </c>
       <c r="B774" t="s">
@@ -24136,7 +24129,7 @@
       </c>
     </row>
     <row r="775" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A775" s="2" t="s">
+      <c r="A775" t="s">
         <v>77</v>
       </c>
       <c r="B775" t="s">
@@ -24168,7 +24161,7 @@
       </c>
     </row>
     <row r="776" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A776" s="2" t="s">
+      <c r="A776" t="s">
         <v>77</v>
       </c>
       <c r="B776" t="s">
@@ -24200,7 +24193,7 @@
       </c>
     </row>
     <row r="777" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A777" s="2" t="s">
+      <c r="A777" t="s">
         <v>77</v>
       </c>
       <c r="B777" t="s">
@@ -24232,7 +24225,7 @@
       </c>
     </row>
     <row r="778" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A778" s="2" t="s">
+      <c r="A778" t="s">
         <v>77</v>
       </c>
       <c r="B778" t="s">
@@ -24264,7 +24257,7 @@
       </c>
     </row>
     <row r="779" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A779" s="2" t="s">
+      <c r="A779" t="s">
         <v>77</v>
       </c>
       <c r="B779" t="s">
@@ -24296,7 +24289,7 @@
       </c>
     </row>
     <row r="780" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A780" s="2" t="s">
+      <c r="A780" t="s">
         <v>77</v>
       </c>
       <c r="B780" t="s">
@@ -24328,7 +24321,7 @@
       </c>
     </row>
     <row r="781" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A781" s="2" t="s">
+      <c r="A781" t="s">
         <v>77</v>
       </c>
       <c r="B781" t="s">
@@ -24360,7 +24353,7 @@
       </c>
     </row>
     <row r="782" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A782" s="2" t="s">
+      <c r="A782" t="s">
         <v>77</v>
       </c>
       <c r="B782" t="s">
@@ -24392,7 +24385,7 @@
       </c>
     </row>
     <row r="784" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A784" s="2" t="s">
+      <c r="A784" t="s">
         <v>78</v>
       </c>
       <c r="B784" t="s">
@@ -24424,7 +24417,7 @@
       </c>
     </row>
     <row r="785" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A785" s="2" t="s">
+      <c r="A785" t="s">
         <v>78</v>
       </c>
       <c r="B785" t="s">
@@ -24456,7 +24449,7 @@
       </c>
     </row>
     <row r="786" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A786" s="2" t="s">
+      <c r="A786" t="s">
         <v>78</v>
       </c>
       <c r="B786" t="s">
@@ -24488,7 +24481,7 @@
       </c>
     </row>
     <row r="787" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A787" s="2" t="s">
+      <c r="A787" t="s">
         <v>78</v>
       </c>
       <c r="B787" t="s">
@@ -24520,7 +24513,7 @@
       </c>
     </row>
     <row r="788" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A788" s="2" t="s">
+      <c r="A788" t="s">
         <v>78</v>
       </c>
       <c r="B788" t="s">
@@ -24552,7 +24545,7 @@
       </c>
     </row>
     <row r="789" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A789" s="2" t="s">
+      <c r="A789" t="s">
         <v>78</v>
       </c>
       <c r="B789" t="s">
@@ -24584,7 +24577,7 @@
       </c>
     </row>
     <row r="790" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A790" s="2" t="s">
+      <c r="A790" t="s">
         <v>78</v>
       </c>
       <c r="B790" t="s">
@@ -24616,7 +24609,7 @@
       </c>
     </row>
     <row r="791" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A791" s="2" t="s">
+      <c r="A791" t="s">
         <v>78</v>
       </c>
       <c r="B791" t="s">
@@ -24648,7 +24641,7 @@
       </c>
     </row>
     <row r="792" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A792" s="2" t="s">
+      <c r="A792" t="s">
         <v>78</v>
       </c>
       <c r="B792" t="s">
@@ -24680,7 +24673,7 @@
       </c>
     </row>
     <row r="793" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A793" s="2" t="s">
+      <c r="A793" t="s">
         <v>78</v>
       </c>
       <c r="B793" t="s">
@@ -24712,7 +24705,7 @@
       </c>
     </row>
     <row r="794" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A794" s="2" t="s">
+      <c r="A794" t="s">
         <v>78</v>
       </c>
       <c r="B794" t="s">
@@ -24744,7 +24737,7 @@
       </c>
     </row>
     <row r="795" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A795" s="2" t="s">
+      <c r="A795" t="s">
         <v>78</v>
       </c>
       <c r="B795" t="s">
@@ -24776,7 +24769,7 @@
       </c>
     </row>
     <row r="796" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A796" s="2" t="s">
+      <c r="A796" t="s">
         <v>78</v>
       </c>
       <c r="B796" t="s">
@@ -24808,7 +24801,7 @@
       </c>
     </row>
     <row r="797" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A797" s="2" t="s">
+      <c r="A797" t="s">
         <v>78</v>
       </c>
       <c r="B797" t="s">
@@ -24840,7 +24833,7 @@
       </c>
     </row>
     <row r="798" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A798" s="2" t="s">
+      <c r="A798" t="s">
         <v>78</v>
       </c>
       <c r="B798" t="s">
@@ -24872,7 +24865,7 @@
       </c>
     </row>
     <row r="799" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A799" s="2" t="s">
+      <c r="A799" t="s">
         <v>78</v>
       </c>
       <c r="B799" t="s">
@@ -24904,7 +24897,7 @@
       </c>
     </row>
     <row r="801" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A801" s="2" t="s">
+      <c r="A801" t="s">
         <v>79</v>
       </c>
       <c r="B801" t="s">
@@ -24936,7 +24929,7 @@
       </c>
     </row>
     <row r="802" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A802" s="2" t="s">
+      <c r="A802" t="s">
         <v>79</v>
       </c>
       <c r="B802" t="s">
@@ -24968,7 +24961,7 @@
       </c>
     </row>
     <row r="803" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A803" s="2" t="s">
+      <c r="A803" t="s">
         <v>79</v>
       </c>
       <c r="B803" t="s">
@@ -25000,7 +24993,7 @@
       </c>
     </row>
     <row r="804" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A804" s="2" t="s">
+      <c r="A804" t="s">
         <v>79</v>
       </c>
       <c r="B804" t="s">
@@ -25032,7 +25025,7 @@
       </c>
     </row>
     <row r="805" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A805" s="2" t="s">
+      <c r="A805" t="s">
         <v>79</v>
       </c>
       <c r="B805" t="s">
@@ -25064,7 +25057,7 @@
       </c>
     </row>
     <row r="806" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A806" s="2" t="s">
+      <c r="A806" t="s">
         <v>79</v>
       </c>
       <c r="B806" t="s">
@@ -25096,7 +25089,7 @@
       </c>
     </row>
     <row r="807" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A807" s="2" t="s">
+      <c r="A807" t="s">
         <v>79</v>
       </c>
       <c r="B807" t="s">
@@ -25128,7 +25121,7 @@
       </c>
     </row>
     <row r="808" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A808" s="2" t="s">
+      <c r="A808" t="s">
         <v>79</v>
       </c>
       <c r="B808" t="s">
@@ -25160,7 +25153,7 @@
       </c>
     </row>
     <row r="809" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A809" s="2" t="s">
+      <c r="A809" t="s">
         <v>79</v>
       </c>
       <c r="B809" t="s">
@@ -25192,7 +25185,7 @@
       </c>
     </row>
     <row r="810" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A810" s="2" t="s">
+      <c r="A810" t="s">
         <v>79</v>
       </c>
       <c r="B810" t="s">
@@ -25224,7 +25217,7 @@
       </c>
     </row>
     <row r="811" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A811" s="2" t="s">
+      <c r="A811" t="s">
         <v>79</v>
       </c>
       <c r="B811" t="s">
@@ -25256,7 +25249,7 @@
       </c>
     </row>
     <row r="812" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A812" s="2" t="s">
+      <c r="A812" t="s">
         <v>79</v>
       </c>
       <c r="B812" t="s">
@@ -25288,7 +25281,7 @@
       </c>
     </row>
     <row r="813" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A813" s="2" t="s">
+      <c r="A813" t="s">
         <v>79</v>
       </c>
       <c r="B813" t="s">
@@ -25320,7 +25313,7 @@
       </c>
     </row>
     <row r="814" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A814" s="2" t="s">
+      <c r="A814" t="s">
         <v>79</v>
       </c>
       <c r="B814" t="s">
@@ -25352,7 +25345,7 @@
       </c>
     </row>
     <row r="815" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A815" s="2" t="s">
+      <c r="A815" t="s">
         <v>79</v>
       </c>
       <c r="B815" t="s">
@@ -25384,7 +25377,7 @@
       </c>
     </row>
     <row r="816" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A816" s="2" t="s">
+      <c r="A816" t="s">
         <v>79</v>
       </c>
       <c r="B816" t="s">

</xml_diff>